<commit_message>
fix(export): Move hyperlinks to article_id instead of title for better readability
- Change format from: article_id | HYPERLINK(title) | date | newspaper
- To: HYPERLINK(article_id) | title | date | newspaper
- Improves readability of press articles in Presse column

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/outputs/export_final_40_personnes.xlsx
+++ b/outputs/export_final_40_personnes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="264">
   <si>
     <t>Nom</t>
   </si>
@@ -749,57 +749,6 @@
   </si>
   <si>
     <t>Conférence de Venise Chambres de commerce</t>
-  </si>
-  <si>
-    <t>IMP-1922-09-27-a-i0029 | =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-27-a-i0029","Bibliographie") | 1922-09-27 | IMP; JDG-1922-09-05-a-i0030 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-05-a-i0030","Assemblées à la Réformation") | 1922-09-05 | JDG; JDG-1922-09-06-a-i0010 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-06-a-i0010","Lettre de Finlande") | 1922-09-06 | JDG; JDG-1922-09-28-a-i0045 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-28-a-i0045","[Sans titre]") | 1922-09-28 | JDG; lepetitparisien-1922-08-18-a-i0044 | =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-18-a-i0044","LE XIV3 CONGRÈS UNIVERSEL D'ESPERANTO") | 1922-08-18 | lepetitparisien; LLS-1922-10-21-a-i0025 | =HYPERLINK("https://impresso-project.ch/app/article/LLS-1922-10-21-a-i0025","Vient de paraître") | 1922-10-21 | LLS; LLS-1922-10-07-a-i0020 | =HYPERLINK("https://impresso-project.ch/app/article/LLS-1922-10-07-a-i0020","Vient de paraître") | 1922-10-07 | LLS; JDG-1922-09-30-a-i0047 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-30-a-i0047","PARTI DÉMOCRATIQUE") | 1922-09-30 | JDG; LSE-1922-09-25-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-09-25-a-i0001","Quotidien socialiste Lecteurs, I’ î socialiste est paru Vive la Démocr[...]") | 1922-09-25 | LSE; NZZ-1922-09-07-b-i0006 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-07-b-i0006","[Sans titre]") | 1922-09-07 | NZZ; LSE-1922-09-22-a-i0025 | =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-09-22-a-i0025","ETRANGER") | 1922-09-22 | LSE; GDL-1922-10-29-a-i0072 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-10-29-a-i0072","LES LIVRES DU JOUR") | 1922-10-29 | GDL</t>
-  </si>
-  <si>
-    <t>JDG-1922-09-17-a-i0021 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-17-a-i0021","[Sans titre]") | 1922-09-17 | JDG; GDL-1922-09-17-a-i0010 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-17-a-i0010","Sa Sfs Ma") | 1922-09-17 | GDL; oeuvre-1922-09-09-a-i0027 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-09-a-i0027","UN GRAND DISCOURS DE LORD BALFOUR") | 1922-09-09 | oeuvre; JDG-1922-08-06-a-i0004 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-06-a-i0004","Sous les ombrages d'Academus") | 1922-08-06 | JDG; lepetitparisien-1922-09-06-a-i0027 | =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-09-06-a-i0027","La troisième séance de l'Assemblée de la S. D. H") | 1922-09-06 | lepetitparisien; JDG-1922-08-02-a-i0020 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-02-a-i0020","Le proche Orient") | 1922-08-02 | JDG; JDG-1922-09-13-a-i0092 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-13-a-i0092","gme Société des nations") | 1922-09-13 | JDG; GDL-1922-09-22-a-i0079 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-22-a-i0079","La troisième session delaJU. N.") | 1922-09-22 | GDL; JDG-1922-09-06-a-i0025 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-06-a-i0025","LA QUATRIEME SEANCE") | 1922-09-06 | JDG; GDL-1922-09-29-a-i0004 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-29-a-i0004","La troisième session de la S. d. N. Vingtième séance plénière") | 1922-09-29 | GDL; JDG-1922-09-22-a-i0029 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-22-a-i0029","Contre l'esclavage") | 1922-09-22 | JDG; JDG-1922-09-07-a-i0015 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-07-a-i0015","Société des nations") | 1922-09-07 | JDG; indeplux-1922-09-13-a-i0039 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-13-a-i0039","Société des Nations La Société des Nations au travail") | 1922-09-13 | indeplux; oeuvre-1922-09-22-a-i0093 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-22-a-i0093","L'ASSEMBLÉE DE LA SOCIÉTÉ DES NATIONS s'occupe de la protection des mi[...]") | 1922-09-22 | oeuvre; oeuvre-1922-09-15-a-i0030 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-15-a-i0030","A GENÈVE, PENDANT L'ENTR'ACTE : Le projet de Lord Robert Cecil a fait [...]") | 1922-09-15 | oeuvre; LSE-1922-10-11-a-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-10-11-a-i0002","EN EUROPE CENTRALE Aux Chambres féd") | 1922-10-11 | LSE; GDL-1922-08-03-a-i0012 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-03-a-i0012","Sa fia. Ni") | 1922-08-03 | GDL; NZZ-1922-09-23-a-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-23-a-i0002","[Sans titre]") | 1922-09-23 | NZZ; LSE-1922-09-15-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-09-15-a-i0001","Quotidien socialiste |OT~Citoyens suisses, ne vous laissez pas museler[...]") | 1922-09-15 | LSE; GDL-1922-09-14-a-i0011 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-14-a-i0011","9B ÊEB NB") | 1922-09-14 | GDL; NZZ-1922-09-29-c-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-29-c-i0002","[Sans titre]") | 1922-09-29 | NZZ; LSE-1922-10-10-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-10-10-a-i0001","La Sentinelle Quotidien socialiste Lecteurs, achetez de préférence l’Â[...]") | 1922-10-10 | LSE; NZZ-1922-09-21-a-i0010 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-21-a-i0010","[Sans titre]") | 1922-09-21 | NZZ; NZZ-1922-09-21-a-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-21-a-i0002","[Sans titre]") | 1922-09-21 | NZZ; NZZ-1922-09-15-b-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-15-b-i0001","[Sans titre]") | 1922-09-15 | NZZ; NZZ-1922-09-11-b-i0014 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-11-b-i0014","[Sans titre]") | 1922-09-11 | NZZ; NZZ-1922-09-26-c-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-26-c-i0002","[Sans titre]") | 1922-09-26 | NZZ; LLE-1922-09-07-a-i0006 | =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-09-07-a-i0006","Société des nations") | 1922-09-07 | LLE</t>
-  </si>
-  <si>
-    <t>JDG-1922-08-21-a-i0029 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-21-a-i0029","CARNET DU JOUR") | 1922-08-21 | JDG; LES-1922-08-19-a-i0010 | =HYPERLINK("https://impresso-project.ch/app/article/LES-1922-08-19-a-i0010","Le Bureau International raueaiion") | 1922-08-19 | LES; GDL-1922-08-06-a-i0011 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-06-a-i0011","S&amp;gt; dL ra") | 1922-08-06 | GDL; JDG-1922-08-23-a-i0044 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-23-a-i0044","[Sans titre]") | 1922-08-23 | JDG; JDG-1922-08-20-a-i0054 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-20-a-i0054","CARNET DU JOUR") | 1922-08-20 | JDG; JDG-1922-09-16-a-i0040 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0040","[Sans titre]") | 1922-09-16 | JDG; JDG-1922-09-17-a-i0054 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-17-a-i0054","ÛEiÈWE") | 1922-09-17 | JDG; JDG-1922-08-15-a-i0041 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-15-a-i0041","CARNET DU JOUR") | 1922-08-15 | JDG; JDG-1922-08-19-a-i0045 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-19-a-i0045","GENÈVE") | 1922-08-19 | JDG; JDG-1922-08-11-a-i0042 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-11-a-i0042","GENÈV E") | 1922-08-11 | JDG; JDG-1922-08-05-a-i0017 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-05-a-i0017","Société des dations") | 1922-08-05 | JDG; JDG-1922-08-11-a-i0043 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-11-a-i0043","CARNET DU JOUR") | 1922-08-11 | JDG; JDG-1922-08-13-a-i0043 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-13-a-i0043","GENÈVE") | 1922-08-13 | JDG; JDG-1922-08-19-a-i0048 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-19-a-i0048","CARNET DU JOUR") | 1922-08-19 | JDG; NZZ-1922-08-13-d-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-13-d-i0001","[Sans titre]") | 1922-08-13 | NZZ</t>
-  </si>
-  <si>
-    <t>indeplux-1922-10-16-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-10-16-a-i0001","Billet extérieur") | 1922-10-16 | indeplux; indeplux-1922-09-04-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-04-a-i0001","Billet extérieur") | 1922-09-04 | indeplux; indeplux-1922-09-18-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-18-a-i0001","Billet extérieur") | 1922-09-18 | indeplux; indeplux-1922-10-30-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-10-30-a-i0001","Billet extérieur") | 1922-10-30 | indeplux; indeplux-1922-08-16-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-16-a-i0001","Billet extérieur") | 1922-08-16 | indeplux; indeplux-1922-10-23-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-10-23-a-i0001","Billet extérieur") | 1922-10-23 | indeplux; indeplux-1922-10-09-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-10-09-a-i0001","Billet extérieur") | 1922-10-09 | indeplux; indeplux-1922-08-21-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-21-a-i0001","Billet extérieur") | 1922-08-21 | indeplux; indeplux-1922-09-13-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-13-a-i0001","Billet extérieur") | 1922-09-13 | indeplux; indeplux-1922-08-28-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-28-a-i0001","Billet extérieur") | 1922-08-28 | indeplux; indeplux-1922-09-25-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-25-a-i0001","Billet extérieur") | 1922-09-25 | indeplux; indeplux-1922-08-08-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-08-a-i0001","Billet extérieur") | 1922-08-08 | indeplux; EXP-1922-09-02-a-i0094 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-02-a-i0094","POLITIQUE ,") | 1922-09-02 | EXP</t>
-  </si>
-  <si>
-    <t>GDL-1922-08-21-a-i0020 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-21-a-i0020","9B CB Sa") | 1922-08-21 | GDL; indeplux-1922-08-23-a-i0019 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-23-a-i0019","M. Léon Bérard et l’Espéranto") | 1922-08-23 | indeplux; lepetitparisien-1922-08-24-a-i0070 | =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-24-a-i0070","L'ESPÉRANTO") | 1922-08-24 | lepetitparisien; NZZ-1922-09-25-a-i0005 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-25-a-i0005","[Sans titre]") | 1922-09-25 | NZZ</t>
-  </si>
-  <si>
-    <t>EXP-1922-08-24-a-i0049 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-24-a-i0049","POLITIQUE") | 1922-08-24 | EXP; JDG-1922-08-23-a-i0107 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-23-a-i0107","Société des Nations") | 1922-08-23 | JDG</t>
-  </si>
-  <si>
-    <t>EXP-1922-09-13-a-i0069 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-13-a-i0069","POLITIQUE Société des nations") | 1922-09-13 | EXP; JDG-1922-09-13-a-i0020 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-13-a-i0020","Société des nations") | 1922-09-13 | JDG; oecaen-1922-09-20-a-i0031 | =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-09-20-a-i0031","&lt; LA FXiBCHB") | 1922-09-20 | oecaen; oeuvre-1922-09-19-a-i0026 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-19-a-i0026","LA DIXIÈME ASSAMBLEE PLÊNIÈRE") | 1922-09-19 | oeuvre</t>
-  </si>
-  <si>
-    <t>oeuvre-1922-08-05-a-i0034 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-08-05-a-i0034","L'Amérique et la Société des Nations") | 1922-08-05 | oeuvre; GDL-1922-08-17-a-i0074 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-17-a-i0074","[Sans titre]") | 1922-08-17 | GDL; JDG-1922-08-17-a-i0083 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-17-a-i0083","Société des Nations") | 1922-08-17 | JDG; lematin-1922-09-19-a-i0039 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-19-a-i0039","Les secours aux réfugiés de Smyrne") | 1922-09-19 | lematin; JDG-1922-09-10-a-i0016 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-10-a-i0016","DISCUSSIO N GENERAL E SU R L E RAPPOR T D U CONSEI L") | 1922-09-10 | JDG; JDG-1922-10-27-a-i0044 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-10-27-a-i0044","IV me C©nféreisce du îravai") | 1922-10-27 | JDG; JDG-1922-09-19-a-i0090 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-19-a-i0090","S me EDITION Société des nations") | 1922-09-19 | JDG; EXP-1922-08-18-a-i0035 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-18-a-i0035","POLITIQUE") | 1922-08-18 | EXP; JDG-1922-10-02-a-i0020 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-10-02-a-i0020","Société des nations") | 1922-10-02 | JDG; GDL-1922-09-04-a-i0071 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-04-a-i0071","Sa da") | 1922-09-04 | GDL; legaulois-1922-10-03-a-i0004 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-10-03-a-i0004","DANS LE MONDE OFFICIEL") | 1922-10-03 | legaulois; EXP-1922-09-04-a-i0056 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-04-a-i0056","APOLITIQUE") | 1922-09-04 | EXP; GDL-1922-09-29-a-i0010 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-29-a-i0010","L'Azerbaïdjan et la S. d.") | 1922-09-29 | GDL; NZZ-1922-09-19-a-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-19-a-i0002","[Sans titre]") | 1922-09-19 | NZZ; LLE-1922-09-05-a-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-09-05-a-i0002","La troisième assemblée de la Société des...") | 1922-09-05 | LLE; luxwort-1922-09-05-a-i0058 | =HYPERLINK("https://impresso-project.ch/app/article/luxwort-1922-09-05-a-i0058","Die 3. Völkerbundsversammlung in Genf.") | 1922-09-05 | luxwort; NZZ-1922-09-03-a-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-03-a-i0002","[Sans titre]") | 1922-09-03 | NZZ; FZG-1922-08-18-a-i0038 | =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-08-18-a-i0038","«danken die schwerste «Niederlage. «Gin ...") | 1922-08-18 | FZG; NZZ-1922-10-23-d-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-10-23-d-i0001","[Sans titre]") | 1922-10-23 | NZZ; FZG-1922-10-24-a-i0014 | =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-10-24-a-i0014","mmmm W&gt;/AL- rMsh*.*.*» A. •*&amp; Jts-**i") | 1922-10-24 | FZG; NZZ-1922-09-03-a-i0009 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-03-a-i0009","[Sans titre]") | 1922-09-03 | NZZ; FZG-1922-09-04-a-i0015 | =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-09-04-a-i0015","• Neueste Meldunam #") | 1922-09-04 | FZG; FZG-1922-09-02-a-i0022 | =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-09-02-a-i0022","Jum griechisch«türkische Konflikt. Adana...") | 1922-09-02 | FZG</t>
-  </si>
-  <si>
-    <t>indeplux-1922-09-22-a-i0018 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-22-a-i0018","Société des Nations Une note exprimant les vœux de la France sera prés[...]") | 1922-09-22 | indeplux; legaulois-1922-09-12-a-i0025 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-12-a-i0025","Réponse de lord Robert Cecil") | 1922-09-12 | legaulois; oeuvre-1922-09-14-a-i0036 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-14-a-i0036","M. LLOYD GEORGE VIENDRA-T-IL A GENÈVE ?") | 1922-09-14 | oeuvre; EXP-1922-09-08-a-i0066 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-08-a-i0066","POLITIQUE Société des Nations") | 1922-09-08 | EXP; oeuvre-1922-10-08-a-i0033 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-10-08-a-i0033","Le Dr Nansen organise une mission purement britannique") | 1922-10-08 | oeuvre; oeuvre-1922-09-20-a-i0027 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-20-a-i0027","LE PROBLÈME DES RÉPARATIONS") | 1922-09-20 | oeuvre; legaulois-1922-09-23-a-i0032 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-23-a-i0032","A LA SOCIÉTÉ DES MATIONS") | 1922-09-23 | legaulois; legaulois-1922-09-01-a-i0016 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-01-a-i0016","Dernière Heure Â la Société des Nations") | 1922-09-01 | legaulois; indeplux-1922-09-14-a-i0046 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-14-a-i0046","Un accord intervient entre lord Robert ( ecil et M. de Jouvenel au suj[...]") | 1922-09-14 | indeplux; indeplux-1922-09-23-a-i0030 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-23-a-i0030","Le point de vue français sur le désarmement") | 1922-09-23 | indeplux; lematin-1922-09-13-a-i0057 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-13-a-i0057","La commission adopté le projet de lord Robert Cecil sur le désarmement") | 1922-09-13 | lematin; JDG-1922-09-09-a-i0010 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0010","LÀ SITUATION") | 1922-09-09 | JDG; JDG-1922-09-08-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-08-a-i0001","BULLETIN") | 1922-09-08 | JDG; legaulois-1922-09-19-a-i0014 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-19-a-i0014","A la Société des Nations") | 1922-09-19 | legaulois; legaulois-1922-09-14-a-i0023 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-14-a-i0023","Vers un pacte de garantie") | 1922-09-14 | legaulois; legaulois-1922-09-07-a-i0045 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-07-a-i0045","Le Chancelier d'Autriche expose la détresse de son pays") | 1922-09-07 | legaulois; lematin-1922-09-23-a-i0037 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-23-a-i0037","LaS.D.N. s'occupe du conflit gréco-turc") | 1922-09-23 | lematin; lepetitparisien-1922-09-12-a-i0032 | =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-09-12-a-i0032","A L'ASSEMBLÉE de la Société des Nations") | 1922-09-12 | lepetitparisien; JDG-1922-09-09-a-i0017 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0017","M. Sciai oj?") | 1922-09-09 | JDG; oeuvre-1922-09-23-a-i0039 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-23-a-i0039","La question d'Orient") | 1922-09-23 | oeuvre; lematin-1922-09-16-a-i0031 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-16-a-i0031","La réduction des armements doit dépendre des garanties données par le [...]") | 1922-09-16 | lematin; EXP-1922-09-18-a-i0049 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-18-a-i0049","1POLITIQUE&amp;gt;£.i") | 1922-09-18 | EXP; IMP-1922-09-12-a-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-12-a-i0002","ba Semaine internationale") | 1922-09-12 | IMP; JDG-1922-09-09-a-i0008 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0008","t&amp;UrcS") | 1922-09-09 | JDG; EXP-1922-10-03-a-i0092 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-10-03-a-i0092","Chronique parlementaire") | 1922-10-03 | EXP; indeplux-1922-09-23-a-i0051 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-23-a-i0051","DERNIÈRE HEURE") | 1922-09-23 | indeplux; IMP-1922-10-03-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-10-03-a-i0001","L&amp;gt;a Semaine internationale") | 1922-10-03 | IMP; lematin-1922-09-17-a-i0038 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-17-a-i0038","Un émouvant débat entre le délégué français et le délégué anglais") | 1922-09-17 | lematin; oeuvre-1922-10-12-a-i0008 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-10-12-a-i0008","M. Lloyd George prépare contre ses détracteurs une grande bataille") | 1922-10-12 | oeuvre; JDG-1922-09-01-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-01-a-i0001","[Sans titre]") | 1922-09-01 | JDG; JDG-1922-09-28-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-28-a-i0001","[Sans titre]") | 1922-09-28 | JDG; EXP-1922-08-23-a-i0043 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-23-a-i0043","POLITIQUE") | 1922-08-23 | EXP; legaulois-1922-09-17-a-i0019 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-17-a-i0019","Dernière A LA SOCIÉTÉ DES NATIONS") | 1922-09-17 | legaulois; legaulois-1922-09-18-a-i0018 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-18-a-i0018","Dernière Heure AU SOCIÉTÉ DES MATIONS") | 1922-09-18 | legaulois; GDL-1922-09-21-a-i0061 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-21-a-i0061","La troisième session de la S. d. N.") | 1922-09-21 | GDL; GDL-1922-09-14-a-i0059 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-14-a-i0059","Chronique de la S. d.N") | 1922-09-14 | GDL; EXP-1922-10-06-a-i0093 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-10-06-a-i0093","Après la session") | 1922-10-06 | EXP; legaulois-1922-09-08-a-i0034 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-08-a-i0034","A LA SOCIÉTÉ DES KATIONS") | 1922-09-08 | legaulois; legaulois-1922-09-12-a-i0024 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-12-a-i0024","A LA SOCIÉTÉ DES NATIONS") | 1922-09-12 | legaulois; lematin-1922-09-13-a-i0077 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-13-a-i0077","LA PROCHAINE ARRIVÉE DE M. LLOYD GEORGE A GENÈVE") | 1922-09-13 | lematin; JDG-1922-09-15-a-i0090 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0090","Le plan Cecil et la doctrine d e Monroë") | 1922-09-15 | JDG; EXP-1922-09-13-a-i0043 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-13-a-i0043","POLITIQUE Société des ffati _ * __§") | 1922-09-13 | EXP; GDL-1922-08-23-a-i0012 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-23-a-i0012","S.") | 1922-08-23 | GDL; JDG-1922-09-15-a-i0006 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0006","BULLETIN") | 1922-09-15 | JDG; JDG-1922-10-05-a-i0006 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-10-05-a-i0006","Chronique parlementaire") | 1922-10-05 | JDG; JDG-1922-09-22-a-i0010 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-22-a-i0010","[Sans titre]") | 1922-09-22 | JDG; EXP-1922-09-13-a-i0074 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-13-a-i0074","DERNIERES REPÊCHES") | 1922-09-13 | EXP; lematin-1922-09-15-a-i0053 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-15-a-i0053","Le délégué français propose, comme première mesure de réduire les dépe[...]") | 1922-09-15 | lematin; EXP-1922-09-22-a-i0051 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-22-a-i0051","Sodttè des nations") | 1922-09-22 | EXP; IMP-1922-09-28-a-i0029 | =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-28-a-i0029","Ledésarmement devant l'Assemblée de Genève") | 1922-09-28 | IMP; legaulois-1922-09-28-a-i0054 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-28-a-i0054","h la Société des gâtions") | 1922-09-28 | legaulois; oeuvre-1922-09-20-a-i0026 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-20-a-i0026","LE PACTE DE GARANTIE") | 1922-09-20 | oeuvre; JDG-1922-09-14-a-i0020 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-14-a-i0020","L'attitude de l'Argentine") | 1922-09-14 | JDG; JDG-1922-09-20-a-i0090 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-20-a-i0090","Société des nations") | 1922-09-20 | JDG; JDG-1922-09-23-a-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0002","GENEVE, 22 septembre 1922 TJX.LETIN") | 1922-09-23 | JDG; JDG-1922-09-16-a-i0073 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0073","2me EDITION....III Société des nations") | 1922-09-16 | JDG; legaulois-1922-09-20-a-i0025 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-20-a-i0025","A LA SOCIÉTÉ DES NATIONS") | 1922-09-20 | legaulois; GDL-1922-09-09-a-i0004 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-09-a-i0004","La troisième session de la S. d. N.") | 1922-09-09 | GDL; lematin-1922-09-14-a-i0050 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-14-a-i0050","Le pacte de garantie n'affectera aucunement les traités de paix") | 1922-09-14 | lematin; JDG-1922-09-17-a-i0113 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-17-a-i0113","gme EDITION ^•.IH.,.1.1.1— i •• - ...M..,,.,— •• '- • IM.-H..MI.III So[...]") | 1922-09-17 | JDG; lepetitparisien-1922-09-03-a-i0039 | =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-09-03-a-i0039","La troisième assemblée de la Société des nations") | 1922-09-03 | lepetitparisien; indeplux-1922-09-14-a-i0043 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-14-a-i0043","La Commission du Désarmement discute la proposition de pacte de garant[...]") | 1922-09-14 | indeplux; indeplux-1922-09-28-a-i0039 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-28-a-i0039","Société des Nations La discussion sur la réduction des armements se po[...]") | 1922-09-28 | indeplux; lematin-1922-09-27-a-i0030 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-27-a-i0030","Quand donc l'humanité ""* , » nous apportant le pacte de garantie, dira[...]") | 1922-09-27 | lematin; oecaen-1922-09-19-a-i0034 | =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-09-19-a-i0034","UN NOUVEAU TEXTE") | 1922-09-19 | oecaen; oecaen-1922-09-27-a-i0006 | =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-09-27-a-i0006","Les travaux de la Commission du Désarmement devant l'Assemblée") | 1922-09-27 | oecaen; JDG-1922-09-13-a-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-13-a-i0002","fc&amp;S") | 1922-09-13 | JDG; GDL-1922-09-27-a-i0004 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-27-a-i0004","La troisième session aelaJjLd.ll. Dix-septième séance plénière") | 1922-09-27 | GDL; legaulois-1922-08-26-a-i0038 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-26-a-i0038","Revue de la Presse") | 1922-08-26 | legaulois; EXP-1922-09-06-a-i0059 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-06-a-i0059","POLITIQUE Société cS@s Nattons") | 1922-09-06 | EXP; lepetitparisien-1922-09-09-a-i0056 | =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-09-09-a-i0056","CE QUE LA FRANCE A FAIT pour diminuer ses armements") | 1922-09-09 | lepetitparisien; indeplux-1922-08-31-a-i0027 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-31-a-i0027","Une proposition de lord Robert Cecil au sujet du désarmement") | 1922-08-31 | indeplux; oeuvre-1922-10-25-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-10-25-a-i0001","POUR QUE L'ENTENTE REDEVIENNE CORDIALE : Définissons nos « buts de pai[...]") | 1922-10-25 | oeuvre; oeuvre-1922-09-23-a-i0038 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-23-a-i0038","Un foyer national pour les Arméniens") | 1922-09-23 | oeuvre; JDG-1922-09-09-a-i0015 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0015","Assemblée de fa Société des nations") | 1922-09-09 | JDG; JDG-1922-09-23-a-i0099 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0099","TROISIEME EDITION La guerre en Asie Mineure et le problème du proche O[...]") | 1922-09-23 | JDG; JDG-1922-09-21-a-i0027 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-21-a-i0027","Dans les Commissions") | 1922-09-21 | JDG; legaulois-1922-09-13-a-i0021 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-13-a-i0021","A LA SOCIÉTÉ DES NATIONS") | 1922-09-13 | legaulois; JDG-1922-09-27-a-i0005 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-27-a-i0005","Assemblée de la Société des nations Séance plénière d") | 1922-09-27 | JDG; EXP-1922-10-28-a-i0069 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-10-28-a-i0069","COÏÏREÎER FRANÇAIS") | 1922-10-28 | EXP; IMP-1922-09-04-a-i0003 | =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-04-a-i0003","Lettre de Genève") | 1922-09-04 | IMP; lematin-1922-09-18-a-i0089 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-18-a-i0089","L'opinion de lord Robert Ceci! sur l'admission du Reich dans la S. D. [...]") | 1922-09-18 | lematin; oecaen-1922-09-18-a-i0016 | =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-09-18-a-i0016","Lord Robert Cecfl est partisan de l'admission de l'Allemagne à la SM.") | 1922-09-18 | oecaen; indeplux-1922-09-06-a-i0012 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-06-a-i0012","L’Assemblée de la S. d. N.") | 1922-09-06 | indeplux; lematin-1922-09-01-a-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-01-a-i0002","M. Lloyd George ira-t-il à Genève?") | 1922-09-01 | lematin; oeuvre-1922-09-21-a-i0038 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-21-a-i0038","Comment la Belgique négociera les bons allemands") | 1922-09-21 | oeuvre; lepetitparisien-1922-10-01-a-i0025 | =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-10-01-a-i0025","LA SOCIÉTÉ DES NATIONS a clos hier ses travaux") | 1922-10-01 | lepetitparisien; indeplux-1922-09-04-a-i0008 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-04-a-i0008","La Commission approuve le projet de lord Robert Cecil sur le desarmeme[...]") | 1922-09-04 | indeplux; legaulois-1922-09-16-a-i0021 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-16-a-i0021","SHAKESPEARE Fils de la Reine Elisabeth") | 1922-09-16 | legaulois; JDG-1922-09-23-a-i0004 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0004","L'Allemagne et ia Société des nations") | 1922-09-23 | JDG; IMP-1922-09-26-a-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-26-a-i0002","ba Semaine internationale") | 1922-09-26 | IMP; legaulois-1922-08-04-a-i0062 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-04-a-i0062","Le débat à la Chambre des Communes") | 1922-08-04 | legaulois; GDL-1922-09-08-a-i0006 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-08-a-i0006","La troisième session de la S. d. N.") | 1922-09-08 | GDL; EXP-1922-09-14-a-i0094 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-14-a-i0094","\. POLITIQUE Société des nations") | 1922-09-14 | EXP; indeplux-1922-09-07-a-i0028 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-07-a-i0028","Un discours de lord Robert Cecil") | 1922-09-07 | indeplux; legaulois-1922-09-15-a-i0026 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-15-a-i0026","Les Journaux du matin") | 1922-09-15 | legaulois; legaulois-1922-09-21-a-i0035 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-21-a-i0035","Les Journaux du matin") | 1922-09-21 | legaulois; GDL-1922-09-18-a-i0060 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-18-a-i0060","9a fia Ni") | 1922-09-18 | GDL; lematin-1922-09-20-a-i0041 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-20-a-i0041","M. de Jouvenel fait, an nom de la délégation française ' I' .. v"" une [...]") | 1922-09-20 | lematin; lematin-1922-10-20-a-i0051 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-10-20-a-i0051","LES GRANDS RETOURS") | 1922-10-20 | lematin; IMP-1922-09-09-a-i0026 | =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-09-a-i0026","Lettre de Genève") | 1922-09-09 | IMP; IMP-1922-09-20-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-20-a-i0001","ba Semaine internationale") | 1922-09-20 | IMP; JDG-1922-09-09-a-i0027 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0027","En marge de l'Assemblée Réceptio n officiell e") | 1922-09-09 | JDG; JDG-1922-09-15-a-i0083 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0083","La guerre en Anatolie et le problème du proche Orient") | 1922-09-15 | JDG; lematin-1922-09-06-a-i0071 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-06-a-i0071","L'assemblée de Genève nomme ses commissions") | 1922-09-06 | lematin</t>
-  </si>
-  <si>
-    <t>legaulois-1922-10-28-a-i0013 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-10-28-a-i0013","NÉCROLOGIE") | 1922-10-28 | legaulois; oecaen-1922-09-26-a-i0049 | =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-09-26-a-i0049","TRIBUNAL CORRECTIONNEL") | 1922-09-26 | oecaen; lepetitparisien-1922-08-22-a-i0053 | =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-22-a-i0053","LECONORÈS UNIVERSEL D'ESPERANTO") | 1922-08-22 | lepetitparisien; lematin-1922-08-08-a-i0074 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-08-a-i0074","NOUVELLES EN TROIS LIGNES") | 1922-08-08 | lematin; oecaen-1922-08-06-a-i0080 | =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-08-06-a-i0080","I !MJbv3") | 1922-08-06 | oecaen</t>
-  </si>
-  <si>
-    <t>indeplux-1922-08-03-a-i0038 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-03-a-i0038","ITALIE La constitution définitive du ministère Facta") | 1922-08-03 | indeplux; GDL-1922-08-02-a-i0013 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-02-a-i0013","Les consultations de M. Facta") | 1922-08-02 | GDL; luxwort-1922-08-03-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/luxwort-1922-08-03-a-i0001","Zur Kabinettsumbildung in Italien.") | 1922-08-03 | luxwort; NZZ-1922-08-01-b-i0006 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-01-b-i0006","[Sans titre]") | 1922-08-01 | NZZ; NZZ-1922-10-18-a-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-10-18-a-i0002","[Sans titre]") | 1922-10-18 | NZZ</t>
-  </si>
-  <si>
-    <t>JDG-1922-10-09-a-i0021 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-10-09-a-i0021","Société des Nations") | 1922-10-09 | JDG</t>
-  </si>
-  <si>
-    <t>LES-1922-08-05-a-i0020 | =HYPERLINK("https://impresso-project.ch/app/article/LES-1922-08-05-a-i0020","Encore si cette revue dépassait par la r...") | 1922-08-05 | LES; JDG-1922-09-16-a-i0036 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0036","A propos du droit d'auteur") | 1922-09-16 | JDG; LCE-1922-09-11-a-i0010 | =HYPERLINK("https://impresso-project.ch/app/article/LCE-1922-09-11-a-i0010","En Suisse Cordages en loysoeoresTravai. Soi C. Kissimg. cordier, Ullle[...]") | 1922-09-11 | LCE; GDL-1922-09-08-a-i0018 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-08-a-i0018","CONFÉDÉRATION") | 1922-09-08 | GDL; NZZ-1922-09-11-b-i0021 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-11-b-i0021","[Sans titre]") | 1922-09-11 | NZZ; NZZ-1922-10-05-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-10-05-a-i0001","[Sans titre]") | 1922-10-05 | NZZ; LLE-1922-09-04-a-i0019 | =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-09-04-a-i0019","Les réformes constitutionnelles au Tessi...") | 1922-09-04 | LLE; FZG-1922-08-26-a-i0017 | =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-08-26-a-i0017","Schweiz") | 1922-08-26 | FZG</t>
-  </si>
-  <si>
-    <t>JDG-1922-08-26-a-i0095 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-26-a-i0095","Nos hôtes") | 1922-08-26 | JDG; lematin-1922-08-06-a-i0076 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-06-a-i0076","Le président de la Confédération helvétique h la Société des nations") | 1922-08-06 | lematin; lematin-1922-09-14-a-i0051 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-14-a-i0051","La coopération intellectuelle") | 1922-09-14 | lematin; legaulois-1922-09-30-a-i0037 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-30-a-i0037","Dernière Heure A LA SOCIÉTÉ DES NATIONS") | 1922-09-30 | legaulois; legaulois-1922-09-14-a-i0018 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-14-a-i0018","A LA SOCIÉTÉ DES NATIONS") | 1922-09-14 | legaulois; legaulois-1922-09-23-a-i0028 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-23-a-i0028","EiteSas lirai»") | 1922-09-23 | legaulois; EXP-1922-09-14-a-i0100 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-14-a-i0100","DERNIERES DEPECHES") | 1922-09-14 | EXP; indeplux-1922-08-29-a-i0081 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-29-a-i0081","Les Fêtes d’Arlon") | 1922-08-29 | indeplux; legaulois-1922-09-29-a-i0025 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-29-a-i0025","A LA SOCIÉTÉ DES HATIONS") | 1922-09-29 | legaulois; GDL-1922-08-28-a-i0055 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-28-a-i0055","LES LIVRES") | 1922-08-28 | GDL; legaulois-1922-08-28-a-i0005 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-28-a-i0005","DANS LES CERCLES") | 1922-08-28 | legaulois; oeuvre-1922-08-04-a-i0025 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-08-04-a-i0025","La défense des ""humanités""") | 1922-08-04 | oeuvre; GDL-1922-08-09-a-i0014 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-09-a-i0014","S. d.") | 1922-08-09 | GDL; JDG-1922-08-07-a-i0003 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-07-a-i0003","Influence de l'habitude") | 1922-08-07 | JDG; JDG-1922-09-05-a-i0003 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-05-a-i0003","Lettre de Paris") | 1922-09-05 | JDG; legaulois-1922-10-06-a-i0056 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-10-06-a-i0056","Les Échos") | 1922-10-06 | legaulois; GDL-1922-09-16-a-i0067 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-16-a-i0067","Chronique de la S. d. N") | 1922-09-16 | GDL; JDG-1922-08-14-a-i0006 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-14-a-i0006","A propos du paradoxe d'Einstein") | 1922-08-14 | JDG; JDG-1922-09-15-a-i0024 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0024","Séance plénière") | 1922-09-15 | JDG; oeuvre-1922-08-16-a-i0067 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-08-16-a-i0067","La Vie philosophique : Durée et simultanéité. A propos de la théorie d[...]") | 1922-08-16 | oeuvre; legaulois-1922-08-06-a-i0008 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-06-a-i0008","PETIT CARNET") | 1922-08-06 | legaulois; JDG-1922-09-16-a-i0020 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0020","Dans les Commissions") | 1922-09-16 | JDG; EXP-1922-08-24-a-i0013 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-24-a-i0013","[Sans titre]") | 1922-08-24 | EXP; lepetitparisien-1922-08-04-a-i0056 | =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-04-a-i0056","LE DONJON DE VINCENNES SEfHUWL TRANSFORME EN BIBLIOTHÈQUE INTERNATIONA[...]") | 1922-08-04 | lepetitparisien; legaulois-1922-10-26-a-i0051 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-10-26-a-i0051","Les Cinq Académies") | 1922-10-26 | legaulois; IMP-1922-08-26-a-i0023 | =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-08-26-a-i0023","Chronique suisse") | 1922-08-26 | IMP; lepetitparisien-1922-08-01-a-i0029 | =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-01-a-i0029","LE COMITÉ DE COOPÉRATION INTELLECTUELLE SE RÉUNIT AUJOURD'HUI A GENÈVE") | 1922-08-01 | lepetitparisien; legaulois-1922-10-13-a-i0034 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-10-13-a-i0034","Les Échos") | 1922-10-13 | legaulois; legaulois-1922-08-04-a-i0023 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-04-a-i0023","Les Échos") | 1922-08-04 | legaulois; legaulois-1922-09-30-a-i0011 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-30-a-i0011","PETIT CARNET") | 1922-09-30 | legaulois; GDL-1922-09-14-a-i0048 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-14-a-i0048","[Sans titre]") | 1922-09-14 | GDL; GDL-1922-09-15-a-i0073 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-15-a-i0073","Chronique de la S. d. N.") | 1922-09-15 | GDL; EXP-1922-08-08-a-i0046 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-08-a-i0046","Coopération intellectuelle") | 1922-08-08 | EXP; GDL-1922-08-02-a-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-02-a-i0002","Deux commissions de premier plan") | 1922-08-02 | GDL; legaulois-1922-08-19-a-i0025 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-19-a-i0025","LES LIVRES DU JOUR") | 1922-08-19 | legaulois; JDG-1922-09-14-a-i0095 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-14-a-i0095","Société des nations XXme session du Conseil") | 1922-09-14 | JDG; oeuvre-1922-09-14-a-i0034 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-14-a-i0034","UN RAPPORT DE M. BERGSON") | 1922-09-14 | oeuvre; EXP-1922-08-10-a-i0021 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-10-a-i0021","[Sans titre]") | 1922-08-10 | EXP; legaulois-1922-08-26-a-i0025 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-26-a-i0025","LES LIVRES DU JOUR") | 1922-08-26 | legaulois; oeuvre-1922-10-06-a-i0016 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-10-06-a-i0016","Les mots en suspens") | 1922-10-06 | oeuvre; obermosel-1922-08-10-a-i0029 | =HYPERLINK("https://impresso-project.ch/app/article/obermosel-1922-08-10-a-i0029","Organisierung der internation. geistigen Arbeit.") | 1922-08-10 | obermosel; lepetitparisien-1922-09-14-a-i0026 | =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-09-14-a-i0026","LA QUESTION DU PACTE DE GARANTIE") | 1922-09-14 | lepetitparisien; oeuvre-1922-09-16-a-i0035 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-16-a-i0035","LA COOPÉRATION INTELLECTUELLE") | 1922-09-16 | oeuvre; LLE-1922-08-02-a-i0006 | =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-08-02-a-i0006","Deux trains allant à Lourdes se tamponne...") | 1922-08-02 | LLE; lematin-1922-08-02-a-i0051 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-02-a-i0051","NOUVELLES EN TROIS LIGNES") | 1922-08-02 | lematin; GDL-1922-08-06-a-i0074 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-06-a-i0074","Sa £••") | 1922-08-06 | GDL; oeuvre-1922-08-02-a-i0085 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-08-02-a-i0085","La Vie philosophique") | 1922-08-02 | oeuvre; GDL-1922-08-26-a-i0026 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-26-a-i0026","CANTON DE VAUD") | 1922-08-26 | GDL; NZZ-1922-09-14-b-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-14-b-i0001","[Sans titre]") | 1922-09-14 | NZZ; LLE-1922-09-16-a-i0090 | =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-09-16-a-i0090","SOCIETE DES NATIONS") | 1922-09-16 | LLE; LLE-1922-08-26-a-i0101 | =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-08-26-a-i0101","Confédération") | 1922-08-26 | LLE; NZZ-1922-08-07-b-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-07-b-i0002","[Sans titre]") | 1922-08-07 | NZZ; NZZ-1922-10-19-b-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-10-19-b-i0001","[Sans titre]") | 1922-10-19 | NZZ; LSE-1922-09-22-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-09-22-a-i0001","Quotidien socialiste") | 1922-09-22 | LSE; JDG-1922-08-06-a-i0040 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-06-a-i0040","[Sans titre]") | 1922-08-06 | JDG; tageblatt-1922-09-15-a-i0010 | =HYPERLINK("https://impresso-project.ch/app/article/tageblatt-1922-09-15-a-i0010","Vom Völkerbund.  Nie intellektuelle Arbeit und der Völkerbund.") | 1922-09-15 | tageblatt; NZZ-1922-08-01-b-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-01-b-i0002","[Sans titre]") | 1922-08-01 | NZZ; GDL-1922-08-01-a-i0064 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-01-a-i0064","S.d. N") | 1922-08-01 | GDL; NZZ-1922-09-14-b-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-14-b-i0002","[Sans titre]") | 1922-09-14 | NZZ; NZZ-1922-08-08-a-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-08-a-i0002","[Sans titre]") | 1922-08-08 | NZZ; LLE-1922-08-09-a-i0007 | =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-08-09-a-i0007","Le comité de coopération Intellectuelle") | 1922-08-09 | LLE; NZZ-1922-08-05-b-i0002 | =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-05-b-i0002","[Sans titre]") | 1922-08-05 | NZZ</t>
-  </si>
-  <si>
-    <t>oeuvre-1922-09-23-a-i0036 | =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-23-a-i0036","Le rapatriement des prisonniers de guerre") | 1922-09-23 | oeuvre; LLE-1922-08-25-a-i0008 | =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-08-25-a-i0008","SOCIÉTÉ DES NATIONS") | 1922-08-25 | LLE; JDG-1922-09-16-a-i0010 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0010","Société des nations") | 1922-09-16 | JDG; JDG-1922-09-20-a-i0001 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-20-a-i0001","[Sans titre]") | 1922-09-20 | JDG; JDG-1922-09-25-a-i0039 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-25-a-i0039","[Sans titre]") | 1922-09-25 | JDG; JDG-1922-09-23-a-i0015 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0015","Assemblée de la Société des nations") | 1922-09-23 | JDG; lepetitparisien-1922-08-24-a-i0030 | =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-24-a-i0030","M. Louis de Brouckère est nommé délégué belge à la S. D. N.") | 1922-08-24 | lepetitparisien; JDG-1922-09-26-a-i0084 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-26-a-i0084","g me EDITION Assemblée de la Société des nations") | 1922-09-26 | JDG; JDG-1922-09-07-a-i0036 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-07-a-i0036","Dans les commissions") | 1922-09-07 | JDG; tageblatt-1922-09-05-a-i0034 | =HYPERLINK("https://impresso-project.ch/app/article/tageblatt-1922-09-05-a-i0034","PETITS COUPS D'ÊPINGLE.") | 1922-09-05 | tageblatt; JDG-1922-09-16-a-i0018 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0018","Un télégramme du Brésil. — Pour la Géorgi e") | 1922-09-16 | JDG; indeplux-1922-08-24-a-i0022 | =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-24-a-i0022","La S. d. N.") | 1922-08-24 | indeplux; JDG-1922-09-27-a-i0042 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-27-a-i0042","L'hommage au soldat belge") | 1922-09-27 | JDG; EXP-1922-09-16-a-i0114 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-16-a-i0114","POLITIQUE") | 1922-09-16 | EXP; JDG-1922-09-21-a-i0090 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-21-a-i0090","Assemblée de la Société des nations") | 1922-09-21 | JDG; lematin-1922-08-08-a-i0046 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-08-a-i0046","Une conférence internationale socialiste à Bruxelles") | 1922-08-08 | lematin; JDG-1922-09-03-a-i0043 | =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-03-a-i0043","Délégués à la troisième assemblée") | 1922-09-03 | JDG; lematin-1922-08-24-a-i0056 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-24-a-i0056","NOUVELLES EN TROIS LIGNES") | 1922-08-24 | lematin; EXP-1922-09-04-a-i0040 | =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-04-a-i0040","; ;•,;. POLITIQUE") | 1922-09-04 | EXP; FZG-1922-09-21-a-i0018 | =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-09-21-a-i0018","• Neueste Meldunge« »") | 1922-09-21 | FZG</t>
-  </si>
-  <si>
-    <t>lematin-1922-08-30-a-i0036 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-30-a-i0036","La Bulgarie envoie une mission secrète à Moscou") | 1922-08-30 | lematin; GDL-1922-08-31-a-i0024 | =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-31-a-i0024","S^a VH &amp;") | 1922-08-31 | GDL; lematin-1922-08-31-a-i0068 | =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-31-a-i0068","M. Todoroff n'ira pas à Moscou") | 1922-08-31 | lematin</t>
-  </si>
-  <si>
-    <t>legaulois-1922-09-28-a-i0009 | =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-28-a-i0009","DANS LE MONDE OFFICIEL") | 1922-09-28 | legaulois</t>
   </si>
   <si>
     <t>Suisse</t>
@@ -1295,17 +1244,18 @@
       <c r="G2" t="s">
         <v>233</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-27-a-i0029","IMP-1922-09-27-a-i0029") | Bibliographie | 1922-09-27 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-05-a-i0030","JDG-1922-09-05-a-i0030") | Assemblées à la Réformation | 1922-09-05 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-06-a-i0010","JDG-1922-09-06-a-i0010") | Lettre de Finlande | 1922-09-06 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-28-a-i0045","JDG-1922-09-28-a-i0045") | [Sans titre] | 1922-09-28 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-18-a-i0044","lepetitparisien-1922-08-18-a-i0044") | LE XIV3 CONGRÈS UNIVERSEL D'ESPERANTO | 1922-08-18 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/LLS-1922-10-21-a-i0025","LLS-1922-10-21-a-i0025") | Vient de paraître | 1922-10-21 | LLS; =HYPERLINK("https://impresso-project.ch/app/article/LLS-1922-10-07-a-i0020","LLS-1922-10-07-a-i0020") | Vient de paraître | 1922-10-07 | LLS; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-30-a-i0047","JDG-1922-09-30-a-i0047") | PARTI DÉMOCRATIQUE | 1922-09-30 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-09-25-a-i0001","LSE-1922-09-25-a-i0001") | Quotidien socialiste Lecteurs, I’ î socialiste est paru Vive la Démocr[...] | 1922-09-25 | LSE; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-07-b-i0006","NZZ-1922-09-07-b-i0006") | [Sans titre] | 1922-09-07 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-09-22-a-i0025","LSE-1922-09-22-a-i0025") | ETRANGER | 1922-09-22 | LSE; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-10-29-a-i0072","GDL-1922-10-29-a-i0072") | LES LIVRES DU JOUR | 1922-10-29 | GDL</f>
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
         <v>244</v>
       </c>
-      <c r="I2" t="s">
-        <v>261</v>
-      </c>
       <c r="J2" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K2" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1330,17 +1280,18 @@
       <c r="G3" t="s">
         <v>233</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-17-a-i0021","JDG-1922-09-17-a-i0021") | [Sans titre] | 1922-09-17 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-17-a-i0010","GDL-1922-09-17-a-i0010") | Sa Sfs Ma | 1922-09-17 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-09-a-i0027","oeuvre-1922-09-09-a-i0027") | UN GRAND DISCOURS DE LORD BALFOUR | 1922-09-09 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-06-a-i0004","JDG-1922-08-06-a-i0004") | Sous les ombrages d'Academus | 1922-08-06 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-09-06-a-i0027","lepetitparisien-1922-09-06-a-i0027") | La troisième séance de l'Assemblée de la S. D. H | 1922-09-06 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-02-a-i0020","JDG-1922-08-02-a-i0020") | Le proche Orient | 1922-08-02 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-13-a-i0092","JDG-1922-09-13-a-i0092") | gme Société des nations | 1922-09-13 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-22-a-i0079","GDL-1922-09-22-a-i0079") | La troisième session delaJU. N. | 1922-09-22 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-06-a-i0025","JDG-1922-09-06-a-i0025") | LA QUATRIEME SEANCE | 1922-09-06 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-29-a-i0004","GDL-1922-09-29-a-i0004") | La troisième session de la S. d. N. Vingtième séance plénière | 1922-09-29 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-22-a-i0029","JDG-1922-09-22-a-i0029") | Contre l'esclavage | 1922-09-22 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-07-a-i0015","JDG-1922-09-07-a-i0015") | Société des nations | 1922-09-07 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-13-a-i0039","indeplux-1922-09-13-a-i0039") | Société des Nations La Société des Nations au travail | 1922-09-13 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-22-a-i0093","oeuvre-1922-09-22-a-i0093") | L'ASSEMBLÉE DE LA SOCIÉTÉ DES NATIONS s'occupe de la protection des mi[...] | 1922-09-22 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-15-a-i0030","oeuvre-1922-09-15-a-i0030") | A GENÈVE, PENDANT L'ENTR'ACTE : Le projet de Lord Robert Cecil a fait [...] | 1922-09-15 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-10-11-a-i0002","LSE-1922-10-11-a-i0002") | EN EUROPE CENTRALE Aux Chambres féd | 1922-10-11 | LSE; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-03-a-i0012","GDL-1922-08-03-a-i0012") | Sa fia. Ni | 1922-08-03 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-23-a-i0002","NZZ-1922-09-23-a-i0002") | [Sans titre] | 1922-09-23 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-09-15-a-i0001","LSE-1922-09-15-a-i0001") | Quotidien socialiste |OT~Citoyens suisses, ne vous laissez pas museler[...] | 1922-09-15 | LSE; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-14-a-i0011","GDL-1922-09-14-a-i0011") | 9B ÊEB NB | 1922-09-14 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-29-c-i0002","NZZ-1922-09-29-c-i0002") | [Sans titre] | 1922-09-29 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-10-10-a-i0001","LSE-1922-10-10-a-i0001") | La Sentinelle Quotidien socialiste Lecteurs, achetez de préférence l’Â[...] | 1922-10-10 | LSE; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-21-a-i0010","NZZ-1922-09-21-a-i0010") | [Sans titre] | 1922-09-21 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-21-a-i0002","NZZ-1922-09-21-a-i0002") | [Sans titre] | 1922-09-21 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-15-b-i0001","NZZ-1922-09-15-b-i0001") | [Sans titre] | 1922-09-15 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-11-b-i0014","NZZ-1922-09-11-b-i0014") | [Sans titre] | 1922-09-11 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-26-c-i0002","NZZ-1922-09-26-c-i0002") | [Sans titre] | 1922-09-26 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-09-07-a-i0006","LLE-1922-09-07-a-i0006") | Société des nations | 1922-09-07 | LLE</f>
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
         <v>245</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>260</v>
+      </c>
+      <c r="K3" t="s">
         <v>262</v>
-      </c>
-      <c r="J3" t="s">
-        <v>277</v>
-      </c>
-      <c r="K3" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1365,17 +1316,18 @@
       <c r="G4" t="s">
         <v>233</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-21-a-i0029","JDG-1922-08-21-a-i0029") | CARNET DU JOUR | 1922-08-21 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/LES-1922-08-19-a-i0010","LES-1922-08-19-a-i0010") | Le Bureau International raueaiion | 1922-08-19 | LES; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-06-a-i0011","GDL-1922-08-06-a-i0011") | S&amp;gt; dL ra | 1922-08-06 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-23-a-i0044","JDG-1922-08-23-a-i0044") | [Sans titre] | 1922-08-23 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-20-a-i0054","JDG-1922-08-20-a-i0054") | CARNET DU JOUR | 1922-08-20 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0040","JDG-1922-09-16-a-i0040") | [Sans titre] | 1922-09-16 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-17-a-i0054","JDG-1922-09-17-a-i0054") | ÛEiÈWE | 1922-09-17 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-15-a-i0041","JDG-1922-08-15-a-i0041") | CARNET DU JOUR | 1922-08-15 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-19-a-i0045","JDG-1922-08-19-a-i0045") | GENÈVE | 1922-08-19 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-11-a-i0042","JDG-1922-08-11-a-i0042") | GENÈV E | 1922-08-11 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-05-a-i0017","JDG-1922-08-05-a-i0017") | Société des dations | 1922-08-05 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-11-a-i0043","JDG-1922-08-11-a-i0043") | CARNET DU JOUR | 1922-08-11 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-13-a-i0043","JDG-1922-08-13-a-i0043") | GENÈVE | 1922-08-13 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-19-a-i0048","JDG-1922-08-19-a-i0048") | CARNET DU JOUR | 1922-08-19 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-13-d-i0001","NZZ-1922-08-13-d-i0001") | [Sans titre] | 1922-08-13 | NZZ</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
         <v>246</v>
       </c>
-      <c r="I4" t="s">
-        <v>263</v>
-      </c>
       <c r="J4" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K4" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1397,17 +1349,18 @@
       <c r="G5" t="s">
         <v>233</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-10-16-a-i0001","indeplux-1922-10-16-a-i0001") | Billet extérieur | 1922-10-16 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-04-a-i0001","indeplux-1922-09-04-a-i0001") | Billet extérieur | 1922-09-04 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-18-a-i0001","indeplux-1922-09-18-a-i0001") | Billet extérieur | 1922-09-18 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-10-30-a-i0001","indeplux-1922-10-30-a-i0001") | Billet extérieur | 1922-10-30 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-16-a-i0001","indeplux-1922-08-16-a-i0001") | Billet extérieur | 1922-08-16 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-10-23-a-i0001","indeplux-1922-10-23-a-i0001") | Billet extérieur | 1922-10-23 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-10-09-a-i0001","indeplux-1922-10-09-a-i0001") | Billet extérieur | 1922-10-09 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-21-a-i0001","indeplux-1922-08-21-a-i0001") | Billet extérieur | 1922-08-21 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-13-a-i0001","indeplux-1922-09-13-a-i0001") | Billet extérieur | 1922-09-13 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-28-a-i0001","indeplux-1922-08-28-a-i0001") | Billet extérieur | 1922-08-28 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-25-a-i0001","indeplux-1922-09-25-a-i0001") | Billet extérieur | 1922-09-25 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-08-a-i0001","indeplux-1922-08-08-a-i0001") | Billet extérieur | 1922-08-08 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-02-a-i0094","EXP-1922-09-02-a-i0094") | POLITIQUE , | 1922-09-02 | EXP</f>
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
         <v>247</v>
       </c>
-      <c r="I5" t="s">
-        <v>264</v>
-      </c>
       <c r="J5" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K5" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1432,17 +1385,18 @@
       <c r="G6" t="s">
         <v>234</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-21-a-i0020","GDL-1922-08-21-a-i0020") | 9B CB Sa | 1922-08-21 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-23-a-i0019","indeplux-1922-08-23-a-i0019") | M. Léon Bérard et l’Espéranto | 1922-08-23 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-24-a-i0070","lepetitparisien-1922-08-24-a-i0070") | L'ESPÉRANTO | 1922-08-24 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-25-a-i0005","NZZ-1922-09-25-a-i0005") | [Sans titre] | 1922-09-25 | NZZ</f>
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
         <v>248</v>
       </c>
-      <c r="I6" t="s">
-        <v>265</v>
-      </c>
       <c r="J6" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K6" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1469,13 +1423,13 @@
       </c>
       <c r="H7" s="2"/>
       <c r="I7" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="J7" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K7" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1499,13 +1453,13 @@
       </c>
       <c r="H8" s="2"/>
       <c r="I8" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="J8" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K8" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1527,17 +1481,18 @@
       <c r="G9" t="s">
         <v>233</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>249</v>
+      <c r="H9" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-24-a-i0049","EXP-1922-08-24-a-i0049") | POLITIQUE | 1922-08-24 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-23-a-i0107","JDG-1922-08-23-a-i0107") | Société des Nations | 1922-08-23 | JDG</f>
+        <v>0</v>
       </c>
       <c r="I9" t="s">
         <v>58</v>
       </c>
       <c r="J9" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K9" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1562,17 +1517,18 @@
       <c r="G10" t="s">
         <v>235</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>250</v>
+      <c r="H10" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-13-a-i0069","EXP-1922-09-13-a-i0069") | POLITIQUE Société des nations | 1922-09-13 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-13-a-i0020","JDG-1922-09-13-a-i0020") | Société des nations | 1922-09-13 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-09-20-a-i0031","oecaen-1922-09-20-a-i0031") | &lt; LA FXiBCHB | 1922-09-20 | oecaen; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-19-a-i0026","oeuvre-1922-09-19-a-i0026") | LA DIXIÈME ASSAMBLEE PLÊNIÈRE | 1922-09-19 | oeuvre</f>
+        <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="J10" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K10" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1599,13 +1555,13 @@
       </c>
       <c r="H11" s="2"/>
       <c r="I11" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="J11" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K11" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1627,17 +1583,18 @@
       <c r="F12" t="s">
         <v>204</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>251</v>
+      <c r="H12" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-08-05-a-i0034","oeuvre-1922-08-05-a-i0034") | L'Amérique et la Société des Nations | 1922-08-05 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-17-a-i0074","GDL-1922-08-17-a-i0074") | [Sans titre] | 1922-08-17 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-17-a-i0083","JDG-1922-08-17-a-i0083") | Société des Nations | 1922-08-17 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-19-a-i0039","lematin-1922-09-19-a-i0039") | Les secours aux réfugiés de Smyrne | 1922-09-19 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-10-a-i0016","JDG-1922-09-10-a-i0016") | DISCUSSIO N GENERAL E SU R L E RAPPOR T D U CONSEI L | 1922-09-10 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-10-27-a-i0044","JDG-1922-10-27-a-i0044") | IV me C©nféreisce du îravai | 1922-10-27 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-19-a-i0090","JDG-1922-09-19-a-i0090") | S me EDITION Société des nations | 1922-09-19 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-18-a-i0035","EXP-1922-08-18-a-i0035") | POLITIQUE | 1922-08-18 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-10-02-a-i0020","JDG-1922-10-02-a-i0020") | Société des nations | 1922-10-02 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-04-a-i0071","GDL-1922-09-04-a-i0071") | Sa da | 1922-09-04 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-10-03-a-i0004","legaulois-1922-10-03-a-i0004") | DANS LE MONDE OFFICIEL | 1922-10-03 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-04-a-i0056","EXP-1922-09-04-a-i0056") | APOLITIQUE | 1922-09-04 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-29-a-i0010","GDL-1922-09-29-a-i0010") | L'Azerbaïdjan et la S. d. | 1922-09-29 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-19-a-i0002","NZZ-1922-09-19-a-i0002") | [Sans titre] | 1922-09-19 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-09-05-a-i0002","LLE-1922-09-05-a-i0002") | La troisième assemblée de la Société des... | 1922-09-05 | LLE; =HYPERLINK("https://impresso-project.ch/app/article/luxwort-1922-09-05-a-i0058","luxwort-1922-09-05-a-i0058") | Die 3. Völkerbundsversammlung in Genf. | 1922-09-05 | luxwort; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-03-a-i0002","NZZ-1922-09-03-a-i0002") | [Sans titre] | 1922-09-03 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-08-18-a-i0038","FZG-1922-08-18-a-i0038") | «danken die schwerste «Niederlage. «Gin ... | 1922-08-18 | FZG; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-10-23-d-i0001","NZZ-1922-10-23-d-i0001") | [Sans titre] | 1922-10-23 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-10-24-a-i0014","FZG-1922-10-24-a-i0014") | mmmm W&gt;/AL- rMsh*.*.*» A. •*&amp; Jts-**i | 1922-10-24 | FZG; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-03-a-i0009","NZZ-1922-09-03-a-i0009") | [Sans titre] | 1922-09-03 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-09-04-a-i0015","FZG-1922-09-04-a-i0015") | • Neueste Meldunam # | 1922-09-04 | FZG; =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-09-02-a-i0022","FZG-1922-09-02-a-i0022") | Jum griechisch«türkische Konflikt. Adana... | 1922-09-02 | FZG</f>
+        <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="J12" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K12" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1662,17 +1619,18 @@
       <c r="G13" t="s">
         <v>233</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>252</v>
+      <c r="H13" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-22-a-i0018","indeplux-1922-09-22-a-i0018") | Société des Nations Une note exprimant les vœux de la France sera prés[...] | 1922-09-22 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-12-a-i0025","legaulois-1922-09-12-a-i0025") | Réponse de lord Robert Cecil | 1922-09-12 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-14-a-i0036","oeuvre-1922-09-14-a-i0036") | M. LLOYD GEORGE VIENDRA-T-IL A GENÈVE ? | 1922-09-14 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-08-a-i0066","EXP-1922-09-08-a-i0066") | POLITIQUE Société des Nations | 1922-09-08 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-10-08-a-i0033","oeuvre-1922-10-08-a-i0033") | Le Dr Nansen organise une mission purement britannique | 1922-10-08 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-20-a-i0027","oeuvre-1922-09-20-a-i0027") | LE PROBLÈME DES RÉPARATIONS | 1922-09-20 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-23-a-i0032","legaulois-1922-09-23-a-i0032") | A LA SOCIÉTÉ DES MATIONS | 1922-09-23 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-01-a-i0016","legaulois-1922-09-01-a-i0016") | Dernière Heure Â la Société des Nations | 1922-09-01 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-14-a-i0046","indeplux-1922-09-14-a-i0046") | Un accord intervient entre lord Robert ( ecil et M. de Jouvenel au suj[...] | 1922-09-14 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-23-a-i0030","indeplux-1922-09-23-a-i0030") | Le point de vue français sur le désarmement | 1922-09-23 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-13-a-i0057","lematin-1922-09-13-a-i0057") | La commission adopté le projet de lord Robert Cecil sur le désarmement | 1922-09-13 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0010","JDG-1922-09-09-a-i0010") | LÀ SITUATION | 1922-09-09 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-08-a-i0001","JDG-1922-09-08-a-i0001") | BULLETIN | 1922-09-08 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-19-a-i0014","legaulois-1922-09-19-a-i0014") | A la Société des Nations | 1922-09-19 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-14-a-i0023","legaulois-1922-09-14-a-i0023") | Vers un pacte de garantie | 1922-09-14 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-07-a-i0045","legaulois-1922-09-07-a-i0045") | Le Chancelier d'Autriche expose la détresse de son pays | 1922-09-07 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-23-a-i0037","lematin-1922-09-23-a-i0037") | LaS.D.N. s'occupe du conflit gréco-turc | 1922-09-23 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-09-12-a-i0032","lepetitparisien-1922-09-12-a-i0032") | A L'ASSEMBLÉE de la Société des Nations | 1922-09-12 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0017","JDG-1922-09-09-a-i0017") | M. Sciai oj? | 1922-09-09 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-23-a-i0039","oeuvre-1922-09-23-a-i0039") | La question d'Orient | 1922-09-23 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-16-a-i0031","lematin-1922-09-16-a-i0031") | La réduction des armements doit dépendre des garanties données par le [...] | 1922-09-16 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-18-a-i0049","EXP-1922-09-18-a-i0049") | 1POLITIQUE&amp;gt;£.i | 1922-09-18 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-12-a-i0002","IMP-1922-09-12-a-i0002") | ba Semaine internationale | 1922-09-12 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0008","JDG-1922-09-09-a-i0008") | t&amp;UrcS | 1922-09-09 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-10-03-a-i0092","EXP-1922-10-03-a-i0092") | Chronique parlementaire | 1922-10-03 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-23-a-i0051","indeplux-1922-09-23-a-i0051") | DERNIÈRE HEURE | 1922-09-23 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-10-03-a-i0001","IMP-1922-10-03-a-i0001") | L&amp;gt;a Semaine internationale | 1922-10-03 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-17-a-i0038","lematin-1922-09-17-a-i0038") | Un émouvant débat entre le délégué français et le délégué anglais | 1922-09-17 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-10-12-a-i0008","oeuvre-1922-10-12-a-i0008") | M. Lloyd George prépare contre ses détracteurs une grande bataille | 1922-10-12 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-01-a-i0001","JDG-1922-09-01-a-i0001") | [Sans titre] | 1922-09-01 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-28-a-i0001","JDG-1922-09-28-a-i0001") | [Sans titre] | 1922-09-28 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-23-a-i0043","EXP-1922-08-23-a-i0043") | POLITIQUE | 1922-08-23 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-17-a-i0019","legaulois-1922-09-17-a-i0019") | Dernière A LA SOCIÉTÉ DES NATIONS | 1922-09-17 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-18-a-i0018","legaulois-1922-09-18-a-i0018") | Dernière Heure AU SOCIÉTÉ DES MATIONS | 1922-09-18 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-21-a-i0061","GDL-1922-09-21-a-i0061") | La troisième session de la S. d. N. | 1922-09-21 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-14-a-i0059","GDL-1922-09-14-a-i0059") | Chronique de la S. d.N | 1922-09-14 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-10-06-a-i0093","EXP-1922-10-06-a-i0093") | Après la session | 1922-10-06 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-08-a-i0034","legaulois-1922-09-08-a-i0034") | A LA SOCIÉTÉ DES KATIONS | 1922-09-08 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-12-a-i0024","legaulois-1922-09-12-a-i0024") | A LA SOCIÉTÉ DES NATIONS | 1922-09-12 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-13-a-i0077","lematin-1922-09-13-a-i0077") | LA PROCHAINE ARRIVÉE DE M. LLOYD GEORGE A GENÈVE | 1922-09-13 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0090","JDG-1922-09-15-a-i0090") | Le plan Cecil et la doctrine d e Monroë | 1922-09-15 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-13-a-i0043","EXP-1922-09-13-a-i0043") | POLITIQUE Société des ffati _ * __§ | 1922-09-13 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-23-a-i0012","GDL-1922-08-23-a-i0012") | S. | 1922-08-23 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0006","JDG-1922-09-15-a-i0006") | BULLETIN | 1922-09-15 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-10-05-a-i0006","JDG-1922-10-05-a-i0006") | Chronique parlementaire | 1922-10-05 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-22-a-i0010","JDG-1922-09-22-a-i0010") | [Sans titre] | 1922-09-22 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-13-a-i0074","EXP-1922-09-13-a-i0074") | DERNIERES REPÊCHES | 1922-09-13 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-15-a-i0053","lematin-1922-09-15-a-i0053") | Le délégué français propose, comme première mesure de réduire les dépe[...] | 1922-09-15 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-22-a-i0051","EXP-1922-09-22-a-i0051") | Sodttè des nations | 1922-09-22 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-28-a-i0029","IMP-1922-09-28-a-i0029") | Ledésarmement devant l'Assemblée de Genève | 1922-09-28 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-28-a-i0054","legaulois-1922-09-28-a-i0054") | h la Société des gâtions | 1922-09-28 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-20-a-i0026","oeuvre-1922-09-20-a-i0026") | LE PACTE DE GARANTIE | 1922-09-20 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-14-a-i0020","JDG-1922-09-14-a-i0020") | L'attitude de l'Argentine | 1922-09-14 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-20-a-i0090","JDG-1922-09-20-a-i0090") | Société des nations | 1922-09-20 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0002","JDG-1922-09-23-a-i0002") | GENEVE, 22 septembre 1922 TJX.LETIN | 1922-09-23 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0073","JDG-1922-09-16-a-i0073") | 2me EDITION....III Société des nations | 1922-09-16 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-20-a-i0025","legaulois-1922-09-20-a-i0025") | A LA SOCIÉTÉ DES NATIONS | 1922-09-20 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-09-a-i0004","GDL-1922-09-09-a-i0004") | La troisième session de la S. d. N. | 1922-09-09 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-14-a-i0050","lematin-1922-09-14-a-i0050") | Le pacte de garantie n'affectera aucunement les traités de paix | 1922-09-14 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-17-a-i0113","JDG-1922-09-17-a-i0113") | gme EDITION ^•.IH.,.1.1.1— i •• - ...M..,,.,— •• '- • IM.-H..MI.III So[...] | 1922-09-17 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-09-03-a-i0039","lepetitparisien-1922-09-03-a-i0039") | La troisième assemblée de la Société des nations | 1922-09-03 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-14-a-i0043","indeplux-1922-09-14-a-i0043") | La Commission du Désarmement discute la proposition de pacte de garant[...] | 1922-09-14 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-28-a-i0039","indeplux-1922-09-28-a-i0039") | Société des Nations La discussion sur la réduction des armements se po[...] | 1922-09-28 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-27-a-i0030","lematin-1922-09-27-a-i0030") | Quand donc l'humanité "* , » nous apportant le pacte de garantie, dira[...] | 1922-09-27 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-09-19-a-i0034","oecaen-1922-09-19-a-i0034") | UN NOUVEAU TEXTE | 1922-09-19 | oecaen; =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-09-27-a-i0006","oecaen-1922-09-27-a-i0006") | Les travaux de la Commission du Désarmement devant l'Assemblée | 1922-09-27 | oecaen; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-13-a-i0002","JDG-1922-09-13-a-i0002") | fc&amp;S | 1922-09-13 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-27-a-i0004","GDL-1922-09-27-a-i0004") | La troisième session aelaJjLd.ll. Dix-septième séance plénière | 1922-09-27 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-26-a-i0038","legaulois-1922-08-26-a-i0038") | Revue de la Presse | 1922-08-26 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-06-a-i0059","EXP-1922-09-06-a-i0059") | POLITIQUE Société cS@s Nattons | 1922-09-06 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-09-09-a-i0056","lepetitparisien-1922-09-09-a-i0056") | CE QUE LA FRANCE A FAIT pour diminuer ses armements | 1922-09-09 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-31-a-i0027","indeplux-1922-08-31-a-i0027") | Une proposition de lord Robert Cecil au sujet du désarmement | 1922-08-31 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-10-25-a-i0001","oeuvre-1922-10-25-a-i0001") | POUR QUE L'ENTENTE REDEVIENNE CORDIALE : Définissons nos « buts de pai[...] | 1922-10-25 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-23-a-i0038","oeuvre-1922-09-23-a-i0038") | Un foyer national pour les Arméniens | 1922-09-23 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0015","JDG-1922-09-09-a-i0015") | Assemblée de fa Société des nations | 1922-09-09 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0099","JDG-1922-09-23-a-i0099") | TROISIEME EDITION La guerre en Asie Mineure et le problème du proche O[...] | 1922-09-23 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-21-a-i0027","JDG-1922-09-21-a-i0027") | Dans les Commissions | 1922-09-21 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-13-a-i0021","legaulois-1922-09-13-a-i0021") | A LA SOCIÉTÉ DES NATIONS | 1922-09-13 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-27-a-i0005","JDG-1922-09-27-a-i0005") | Assemblée de la Société des nations Séance plénière d | 1922-09-27 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-10-28-a-i0069","EXP-1922-10-28-a-i0069") | COÏÏREÎER FRANÇAIS | 1922-10-28 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-04-a-i0003","IMP-1922-09-04-a-i0003") | Lettre de Genève | 1922-09-04 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-18-a-i0089","lematin-1922-09-18-a-i0089") | L'opinion de lord Robert Ceci! sur l'admission du Reich dans la S. D. [...] | 1922-09-18 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-09-18-a-i0016","oecaen-1922-09-18-a-i0016") | Lord Robert Cecfl est partisan de l'admission de l'Allemagne à la SM. | 1922-09-18 | oecaen; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-06-a-i0012","indeplux-1922-09-06-a-i0012") | L’Assemblée de la S. d. N. | 1922-09-06 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-01-a-i0002","lematin-1922-09-01-a-i0002") | M. Lloyd George ira-t-il à Genève? | 1922-09-01 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-21-a-i0038","oeuvre-1922-09-21-a-i0038") | Comment la Belgique négociera les bons allemands | 1922-09-21 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-10-01-a-i0025","lepetitparisien-1922-10-01-a-i0025") | LA SOCIÉTÉ DES NATIONS a clos hier ses travaux | 1922-10-01 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-04-a-i0008","indeplux-1922-09-04-a-i0008") | La Commission approuve le projet de lord Robert Cecil sur le desarmeme[...] | 1922-09-04 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-16-a-i0021","legaulois-1922-09-16-a-i0021") | SHAKESPEARE Fils de la Reine Elisabeth | 1922-09-16 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0004","JDG-1922-09-23-a-i0004") | L'Allemagne et ia Société des nations | 1922-09-23 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-26-a-i0002","IMP-1922-09-26-a-i0002") | ba Semaine internationale | 1922-09-26 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-04-a-i0062","legaulois-1922-08-04-a-i0062") | Le débat à la Chambre des Communes | 1922-08-04 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-08-a-i0006","GDL-1922-09-08-a-i0006") | La troisième session de la S. d. N. | 1922-09-08 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-14-a-i0094","EXP-1922-09-14-a-i0094") | \. POLITIQUE Société des nations | 1922-09-14 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-07-a-i0028","indeplux-1922-09-07-a-i0028") | Un discours de lord Robert Cecil | 1922-09-07 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-15-a-i0026","legaulois-1922-09-15-a-i0026") | Les Journaux du matin | 1922-09-15 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-21-a-i0035","legaulois-1922-09-21-a-i0035") | Les Journaux du matin | 1922-09-21 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-18-a-i0060","GDL-1922-09-18-a-i0060") | 9a fia Ni | 1922-09-18 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-20-a-i0041","lematin-1922-09-20-a-i0041") | M. de Jouvenel fait, an nom de la délégation française ' I' .. v" une [...] | 1922-09-20 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-10-20-a-i0051","lematin-1922-10-20-a-i0051") | LES GRANDS RETOURS | 1922-10-20 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-09-a-i0026","IMP-1922-09-09-a-i0026") | Lettre de Genève | 1922-09-09 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-20-a-i0001","IMP-1922-09-20-a-i0001") | ba Semaine internationale | 1922-09-20 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0027","JDG-1922-09-09-a-i0027") | En marge de l'Assemblée Réceptio n officiell e | 1922-09-09 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0083","JDG-1922-09-15-a-i0083") | La guerre en Anatolie et le problème du proche Orient | 1922-09-15 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-06-a-i0071","lematin-1922-09-06-a-i0071") | L'assemblée de Genève nomme ses commissions | 1922-09-06 | lematin</f>
+        <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="J13" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K13" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1697,17 +1655,18 @@
       <c r="G14" t="s">
         <v>237</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>253</v>
+      <c r="H14" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-10-28-a-i0013","legaulois-1922-10-28-a-i0013") | NÉCROLOGIE | 1922-10-28 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-09-26-a-i0049","oecaen-1922-09-26-a-i0049") | TRIBUNAL CORRECTIONNEL | 1922-09-26 | oecaen; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-22-a-i0053","lepetitparisien-1922-08-22-a-i0053") | LECONORÈS UNIVERSEL D'ESPERANTO | 1922-08-22 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-08-a-i0074","lematin-1922-08-08-a-i0074") | NOUVELLES EN TROIS LIGNES | 1922-08-08 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-08-06-a-i0080","oecaen-1922-08-06-a-i0080") | I !MJbv3 | 1922-08-06 | oecaen</f>
+        <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="J14" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K14" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1734,13 +1693,13 @@
       </c>
       <c r="H15" s="2"/>
       <c r="I15" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="J15" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K15" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1767,13 +1726,13 @@
       </c>
       <c r="H16" s="2"/>
       <c r="I16" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="J16" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K16" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1798,17 +1757,18 @@
       <c r="G17" t="s">
         <v>233</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-03-a-i0038","indeplux-1922-08-03-a-i0038") | ITALIE La constitution définitive du ministère Facta | 1922-08-03 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-02-a-i0013","GDL-1922-08-02-a-i0013") | Les consultations de M. Facta | 1922-08-02 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/luxwort-1922-08-03-a-i0001","luxwort-1922-08-03-a-i0001") | Zur Kabinettsumbildung in Italien. | 1922-08-03 | luxwort; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-01-b-i0006","NZZ-1922-08-01-b-i0006") | [Sans titre] | 1922-08-01 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-10-18-a-i0002","NZZ-1922-10-18-a-i0002") | [Sans titre] | 1922-10-18 | NZZ</f>
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
         <v>254</v>
       </c>
-      <c r="I17" t="s">
-        <v>271</v>
-      </c>
       <c r="J17" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K17" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1838,10 +1798,10 @@
         <v>58</v>
       </c>
       <c r="J18" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K18" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1868,13 +1828,13 @@
       </c>
       <c r="H19" s="2"/>
       <c r="I19" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="J19" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K19" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1898,13 +1858,13 @@
       </c>
       <c r="H20" s="2"/>
       <c r="I20" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="J20" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K20" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1926,17 +1886,18 @@
       <c r="G21" t="s">
         <v>233</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-10-09-a-i0021","JDG-1922-10-09-a-i0021") | Société des Nations | 1922-10-09 | JDG</f>
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
         <v>255</v>
       </c>
-      <c r="I21" t="s">
-        <v>272</v>
-      </c>
       <c r="J21" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K21" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1960,13 +1921,13 @@
       </c>
       <c r="H22" s="2"/>
       <c r="I22" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="J22" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K22" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1990,13 +1951,13 @@
       </c>
       <c r="H23" s="2"/>
       <c r="I23" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="J23" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K23" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -2023,10 +1984,10 @@
         <v>58</v>
       </c>
       <c r="J24" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K24" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2053,13 +2014,13 @@
       </c>
       <c r="H25" s="2"/>
       <c r="I25" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="J25" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K25" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2083,10 +2044,10 @@
         <v>58</v>
       </c>
       <c r="J26" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K26" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -2113,13 +2074,13 @@
       </c>
       <c r="H27" s="2"/>
       <c r="I27" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="J27" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K27" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2141,17 +2102,18 @@
       <c r="G28" t="s">
         <v>235</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>256</v>
+      <c r="H28" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/LES-1922-08-05-a-i0020","LES-1922-08-05-a-i0020") | Encore si cette revue dépassait par la r... | 1922-08-05 | LES; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0036","JDG-1922-09-16-a-i0036") | A propos du droit d'auteur | 1922-09-16 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/LCE-1922-09-11-a-i0010","LCE-1922-09-11-a-i0010") | En Suisse Cordages en loysoeoresTravai. Soi C. Kissimg. cordier, Ullle[...] | 1922-09-11 | LCE; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-08-a-i0018","GDL-1922-09-08-a-i0018") | CONFÉDÉRATION | 1922-09-08 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-11-b-i0021","NZZ-1922-09-11-b-i0021") | [Sans titre] | 1922-09-11 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-10-05-a-i0001","NZZ-1922-10-05-a-i0001") | [Sans titre] | 1922-10-05 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-09-04-a-i0019","LLE-1922-09-04-a-i0019") | Les réformes constitutionnelles au Tessi... | 1922-09-04 | LLE; =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-08-26-a-i0017","FZG-1922-08-26-a-i0017") | Schweiz | 1922-08-26 | FZG</f>
+        <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="J28" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K28" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2176,17 +2138,18 @@
       <c r="G29" t="s">
         <v>240</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>257</v>
+      <c r="H29" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-26-a-i0095","JDG-1922-08-26-a-i0095") | Nos hôtes | 1922-08-26 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-06-a-i0076","lematin-1922-08-06-a-i0076") | Le président de la Confédération helvétique h la Société des nations | 1922-08-06 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-14-a-i0051","lematin-1922-09-14-a-i0051") | La coopération intellectuelle | 1922-09-14 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-30-a-i0037","legaulois-1922-09-30-a-i0037") | Dernière Heure A LA SOCIÉTÉ DES NATIONS | 1922-09-30 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-14-a-i0018","legaulois-1922-09-14-a-i0018") | A LA SOCIÉTÉ DES NATIONS | 1922-09-14 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-23-a-i0028","legaulois-1922-09-23-a-i0028") | EiteSas lirai» | 1922-09-23 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-14-a-i0100","EXP-1922-09-14-a-i0100") | DERNIERES DEPECHES | 1922-09-14 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-29-a-i0081","indeplux-1922-08-29-a-i0081") | Les Fêtes d’Arlon | 1922-08-29 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-29-a-i0025","legaulois-1922-09-29-a-i0025") | A LA SOCIÉTÉ DES HATIONS | 1922-09-29 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-28-a-i0055","GDL-1922-08-28-a-i0055") | LES LIVRES | 1922-08-28 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-28-a-i0005","legaulois-1922-08-28-a-i0005") | DANS LES CERCLES | 1922-08-28 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-08-04-a-i0025","oeuvre-1922-08-04-a-i0025") | La défense des "humanités" | 1922-08-04 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-09-a-i0014","GDL-1922-08-09-a-i0014") | S. d. | 1922-08-09 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-07-a-i0003","JDG-1922-08-07-a-i0003") | Influence de l'habitude | 1922-08-07 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-05-a-i0003","JDG-1922-09-05-a-i0003") | Lettre de Paris | 1922-09-05 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-10-06-a-i0056","legaulois-1922-10-06-a-i0056") | Les Échos | 1922-10-06 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-16-a-i0067","GDL-1922-09-16-a-i0067") | Chronique de la S. d. N | 1922-09-16 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-14-a-i0006","JDG-1922-08-14-a-i0006") | A propos du paradoxe d'Einstein | 1922-08-14 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0024","JDG-1922-09-15-a-i0024") | Séance plénière | 1922-09-15 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-08-16-a-i0067","oeuvre-1922-08-16-a-i0067") | La Vie philosophique : Durée et simultanéité. A propos de la théorie d[...] | 1922-08-16 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-06-a-i0008","legaulois-1922-08-06-a-i0008") | PETIT CARNET | 1922-08-06 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0020","JDG-1922-09-16-a-i0020") | Dans les Commissions | 1922-09-16 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-24-a-i0013","EXP-1922-08-24-a-i0013") | [Sans titre] | 1922-08-24 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-04-a-i0056","lepetitparisien-1922-08-04-a-i0056") | LE DONJON DE VINCENNES SEfHUWL TRANSFORME EN BIBLIOTHÈQUE INTERNATIONA[...] | 1922-08-04 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-10-26-a-i0051","legaulois-1922-10-26-a-i0051") | Les Cinq Académies | 1922-10-26 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-08-26-a-i0023","IMP-1922-08-26-a-i0023") | Chronique suisse | 1922-08-26 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-01-a-i0029","lepetitparisien-1922-08-01-a-i0029") | LE COMITÉ DE COOPÉRATION INTELLECTUELLE SE RÉUNIT AUJOURD'HUI A GENÈVE | 1922-08-01 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-10-13-a-i0034","legaulois-1922-10-13-a-i0034") | Les Échos | 1922-10-13 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-04-a-i0023","legaulois-1922-08-04-a-i0023") | Les Échos | 1922-08-04 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-30-a-i0011","legaulois-1922-09-30-a-i0011") | PETIT CARNET | 1922-09-30 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-14-a-i0048","GDL-1922-09-14-a-i0048") | [Sans titre] | 1922-09-14 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-15-a-i0073","GDL-1922-09-15-a-i0073") | Chronique de la S. d. N. | 1922-09-15 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-08-a-i0046","EXP-1922-08-08-a-i0046") | Coopération intellectuelle | 1922-08-08 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-02-a-i0002","GDL-1922-08-02-a-i0002") | Deux commissions de premier plan | 1922-08-02 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-19-a-i0025","legaulois-1922-08-19-a-i0025") | LES LIVRES DU JOUR | 1922-08-19 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-14-a-i0095","JDG-1922-09-14-a-i0095") | Société des nations XXme session du Conseil | 1922-09-14 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-14-a-i0034","oeuvre-1922-09-14-a-i0034") | UN RAPPORT DE M. BERGSON | 1922-09-14 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-10-a-i0021","EXP-1922-08-10-a-i0021") | [Sans titre] | 1922-08-10 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-26-a-i0025","legaulois-1922-08-26-a-i0025") | LES LIVRES DU JOUR | 1922-08-26 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-10-06-a-i0016","oeuvre-1922-10-06-a-i0016") | Les mots en suspens | 1922-10-06 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/obermosel-1922-08-10-a-i0029","obermosel-1922-08-10-a-i0029") | Organisierung der internation. geistigen Arbeit. | 1922-08-10 | obermosel; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-09-14-a-i0026","lepetitparisien-1922-09-14-a-i0026") | LA QUESTION DU PACTE DE GARANTIE | 1922-09-14 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-16-a-i0035","oeuvre-1922-09-16-a-i0035") | LA COOPÉRATION INTELLECTUELLE | 1922-09-16 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-08-02-a-i0006","LLE-1922-08-02-a-i0006") | Deux trains allant à Lourdes se tamponne... | 1922-08-02 | LLE; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-02-a-i0051","lematin-1922-08-02-a-i0051") | NOUVELLES EN TROIS LIGNES | 1922-08-02 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-06-a-i0074","GDL-1922-08-06-a-i0074") | Sa £•• | 1922-08-06 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-08-02-a-i0085","oeuvre-1922-08-02-a-i0085") | La Vie philosophique | 1922-08-02 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-26-a-i0026","GDL-1922-08-26-a-i0026") | CANTON DE VAUD | 1922-08-26 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-14-b-i0001","NZZ-1922-09-14-b-i0001") | [Sans titre] | 1922-09-14 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-09-16-a-i0090","LLE-1922-09-16-a-i0090") | SOCIETE DES NATIONS | 1922-09-16 | LLE; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-08-26-a-i0101","LLE-1922-08-26-a-i0101") | Confédération | 1922-08-26 | LLE; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-07-b-i0002","NZZ-1922-08-07-b-i0002") | [Sans titre] | 1922-08-07 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-10-19-b-i0001","NZZ-1922-10-19-b-i0001") | [Sans titre] | 1922-10-19 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-09-22-a-i0001","LSE-1922-09-22-a-i0001") | Quotidien socialiste | 1922-09-22 | LSE; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-06-a-i0040","JDG-1922-08-06-a-i0040") | [Sans titre] | 1922-08-06 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/tageblatt-1922-09-15-a-i0010","tageblatt-1922-09-15-a-i0010") | Vom Völkerbund.  Nie intellektuelle Arbeit und der Völkerbund. | 1922-09-15 | tageblatt; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-01-b-i0002","NZZ-1922-08-01-b-i0002") | [Sans titre] | 1922-08-01 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-01-a-i0064","GDL-1922-08-01-a-i0064") | S.d. N | 1922-08-01 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-14-b-i0002","NZZ-1922-09-14-b-i0002") | [Sans titre] | 1922-09-14 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-08-a-i0002","NZZ-1922-08-08-a-i0002") | [Sans titre] | 1922-08-08 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-08-09-a-i0007","LLE-1922-08-09-a-i0007") | Le comité de coopération Intellectuelle | 1922-08-09 | LLE; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-05-b-i0002","NZZ-1922-08-05-b-i0002") | [Sans titre] | 1922-08-05 | NZZ</f>
+        <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="J29" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K29" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -2210,13 +2173,13 @@
       </c>
       <c r="H30" s="2"/>
       <c r="I30" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="J30" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K30" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2243,13 +2206,13 @@
       </c>
       <c r="H31" s="2"/>
       <c r="I31" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="J31" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K31" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2276,10 +2239,10 @@
         <v>58</v>
       </c>
       <c r="J32" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K32" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -2301,17 +2264,18 @@
       <c r="G33" t="s">
         <v>233</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>258</v>
+      <c r="H33" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-23-a-i0036","oeuvre-1922-09-23-a-i0036") | Le rapatriement des prisonniers de guerre | 1922-09-23 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-08-25-a-i0008","LLE-1922-08-25-a-i0008") | SOCIÉTÉ DES NATIONS | 1922-08-25 | LLE; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0010","JDG-1922-09-16-a-i0010") | Société des nations | 1922-09-16 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-20-a-i0001","JDG-1922-09-20-a-i0001") | [Sans titre] | 1922-09-20 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-25-a-i0039","JDG-1922-09-25-a-i0039") | [Sans titre] | 1922-09-25 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0015","JDG-1922-09-23-a-i0015") | Assemblée de la Société des nations | 1922-09-23 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-24-a-i0030","lepetitparisien-1922-08-24-a-i0030") | M. Louis de Brouckère est nommé délégué belge à la S. D. N. | 1922-08-24 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-26-a-i0084","JDG-1922-09-26-a-i0084") | g me EDITION Assemblée de la Société des nations | 1922-09-26 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-07-a-i0036","JDG-1922-09-07-a-i0036") | Dans les commissions | 1922-09-07 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/tageblatt-1922-09-05-a-i0034","tageblatt-1922-09-05-a-i0034") | PETITS COUPS D'ÊPINGLE. | 1922-09-05 | tageblatt; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0018","JDG-1922-09-16-a-i0018") | Un télégramme du Brésil. — Pour la Géorgi e | 1922-09-16 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-24-a-i0022","indeplux-1922-08-24-a-i0022") | La S. d. N. | 1922-08-24 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-27-a-i0042","JDG-1922-09-27-a-i0042") | L'hommage au soldat belge | 1922-09-27 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-16-a-i0114","EXP-1922-09-16-a-i0114") | POLITIQUE | 1922-09-16 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-21-a-i0090","JDG-1922-09-21-a-i0090") | Assemblée de la Société des nations | 1922-09-21 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-08-a-i0046","lematin-1922-08-08-a-i0046") | Une conférence internationale socialiste à Bruxelles | 1922-08-08 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-03-a-i0043","JDG-1922-09-03-a-i0043") | Délégués à la troisième assemblée | 1922-09-03 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-24-a-i0056","lematin-1922-08-24-a-i0056") | NOUVELLES EN TROIS LIGNES | 1922-08-24 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-04-a-i0040","EXP-1922-09-04-a-i0040") | ; ;•,;. POLITIQUE | 1922-09-04 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-09-21-a-i0018","FZG-1922-09-21-a-i0018") | • Neueste Meldunge« » | 1922-09-21 | FZG</f>
+        <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="J33" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K33" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2333,17 +2297,18 @@
       <c r="G34" t="s">
         <v>233</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>259</v>
+      <c r="H34" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-30-a-i0036","lematin-1922-08-30-a-i0036") | La Bulgarie envoie une mission secrète à Moscou | 1922-08-30 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-31-a-i0024","GDL-1922-08-31-a-i0024") | S^a VH &amp; | 1922-08-31 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-31-a-i0068","lematin-1922-08-31-a-i0068") | M. Todoroff n'ira pas à Moscou | 1922-08-31 | lematin</f>
+        <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="J34" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K34" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2370,13 +2335,13 @@
       </c>
       <c r="H35" s="2"/>
       <c r="I35" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="J35" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K35" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2400,10 +2365,10 @@
       </c>
       <c r="H36" s="2"/>
       <c r="I36" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="K36" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2433,10 +2398,10 @@
         <v>58</v>
       </c>
       <c r="J37" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K37" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2460,13 +2425,13 @@
       </c>
       <c r="H38" s="2"/>
       <c r="I38" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="J38" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="K38" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -2490,13 +2455,13 @@
       </c>
       <c r="H39" s="2"/>
       <c r="I39" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="J39" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K39" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2518,17 +2483,18 @@
       <c r="G40" t="s">
         <v>233</v>
       </c>
-      <c r="H40" s="2" t="s">
-        <v>260</v>
+      <c r="H40" s="2">
+        <f>HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-28-a-i0009","legaulois-1922-09-28-a-i0009") | DANS LE MONDE OFFICIEL | 1922-09-28 | legaulois</f>
+        <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="J40" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K40" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2552,13 +2518,13 @@
       </c>
       <c r="H41" s="2"/>
       <c r="I41" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="J41" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="K41" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(export): Fix empty Presse column by using plain URLs instead of HYPERLINK formulas
- Excel cannot handle multiple HYPERLINK formulas in one cell
- Change to format: article_id (url) | titre | date | newspaper
- URLs are visible and clickable in Excel/LibreOffice
- Remove code that was overwriting Presse column
- Increase Presse column width to 100 chars

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/outputs/export_final_40_personnes.xlsx
+++ b/outputs/export_final_40_personnes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="281">
   <si>
     <t>Nom</t>
   </si>
@@ -749,6 +749,57 @@
   </si>
   <si>
     <t>Conférence de Venise Chambres de commerce</t>
+  </si>
+  <si>
+    <t>IMP-1922-09-27-a-i0029 (https://impresso-project.ch/app/article/IMP-1922-09-27-a-i0029) | Bibliographie | 1922-09-27 | IMP; JDG-1922-09-05-a-i0030 (https://impresso-project.ch/app/article/JDG-1922-09-05-a-i0030) | Assemblées à la Réformation | 1922-09-05 | JDG; JDG-1922-09-06-a-i0010 (https://impresso-project.ch/app/article/JDG-1922-09-06-a-i0010) | Lettre de Finlande | 1922-09-06 | JDG; JDG-1922-09-28-a-i0045 (https://impresso-project.ch/app/article/JDG-1922-09-28-a-i0045) | [Sans titre] | 1922-09-28 | JDG; lepetitparisien-1922-08-18-a-i0044 (https://impresso-project.ch/app/article/lepetitparisien-1922-08-18-a-i0044) | LE XIV3 CONGRÈS UNIVERSEL D'ESPERANTO | 1922-08-18 | lepetitparisien; LLS-1922-10-21-a-i0025 (https://impresso-project.ch/app/article/LLS-1922-10-21-a-i0025) | Vient de paraître | 1922-10-21 | LLS; LLS-1922-10-07-a-i0020 (https://impresso-project.ch/app/article/LLS-1922-10-07-a-i0020) | Vient de paraître | 1922-10-07 | LLS; JDG-1922-09-30-a-i0047 (https://impresso-project.ch/app/article/JDG-1922-09-30-a-i0047) | PARTI DÉMOCRATIQUE | 1922-09-30 | JDG; LSE-1922-09-25-a-i0001 (https://impresso-project.ch/app/article/LSE-1922-09-25-a-i0001) | Quotidien socialiste Lecteurs, I’ î socialiste est paru Vive la Démocr[...] | 1922-09-25 | LSE; NZZ-1922-09-07-b-i0006 (https://impresso-project.ch/app/article/NZZ-1922-09-07-b-i0006) | [Sans titre] | 1922-09-07 | NZZ; LSE-1922-09-22-a-i0025 (https://impresso-project.ch/app/article/LSE-1922-09-22-a-i0025) | ETRANGER | 1922-09-22 | LSE; GDL-1922-10-29-a-i0072 (https://impresso-project.ch/app/article/GDL-1922-10-29-a-i0072) | LES LIVRES DU JOUR | 1922-10-29 | GDL</t>
+  </si>
+  <si>
+    <t>JDG-1922-09-17-a-i0021 (https://impresso-project.ch/app/article/JDG-1922-09-17-a-i0021) | [Sans titre] | 1922-09-17 | JDG; GDL-1922-09-17-a-i0010 (https://impresso-project.ch/app/article/GDL-1922-09-17-a-i0010) | Sa Sfs Ma | 1922-09-17 | GDL; oeuvre-1922-09-09-a-i0027 (https://impresso-project.ch/app/article/oeuvre-1922-09-09-a-i0027) | UN GRAND DISCOURS DE LORD BALFOUR | 1922-09-09 | oeuvre; JDG-1922-08-06-a-i0004 (https://impresso-project.ch/app/article/JDG-1922-08-06-a-i0004) | Sous les ombrages d'Academus | 1922-08-06 | JDG; lepetitparisien-1922-09-06-a-i0027 (https://impresso-project.ch/app/article/lepetitparisien-1922-09-06-a-i0027) | La troisième séance de l'Assemblée de la S. D. H | 1922-09-06 | lepetitparisien; JDG-1922-08-02-a-i0020 (https://impresso-project.ch/app/article/JDG-1922-08-02-a-i0020) | Le proche Orient | 1922-08-02 | JDG; JDG-1922-09-13-a-i0092 (https://impresso-project.ch/app/article/JDG-1922-09-13-a-i0092) | gme Société des nations | 1922-09-13 | JDG; GDL-1922-09-22-a-i0079 (https://impresso-project.ch/app/article/GDL-1922-09-22-a-i0079) | La troisième session delaJU. N. | 1922-09-22 | GDL; JDG-1922-09-06-a-i0025 (https://impresso-project.ch/app/article/JDG-1922-09-06-a-i0025) | LA QUATRIEME SEANCE | 1922-09-06 | JDG; GDL-1922-09-29-a-i0004 (https://impresso-project.ch/app/article/GDL-1922-09-29-a-i0004) | La troisième session de la S. d. N. Vingtième séance plénière | 1922-09-29 | GDL; JDG-1922-09-22-a-i0029 (https://impresso-project.ch/app/article/JDG-1922-09-22-a-i0029) | Contre l'esclavage | 1922-09-22 | JDG; JDG-1922-09-07-a-i0015 (https://impresso-project.ch/app/article/JDG-1922-09-07-a-i0015) | Société des nations | 1922-09-07 | JDG; indeplux-1922-09-13-a-i0039 (https://impresso-project.ch/app/article/indeplux-1922-09-13-a-i0039) | Société des Nations La Société des Nations au travail | 1922-09-13 | indeplux; oeuvre-1922-09-22-a-i0093 (https://impresso-project.ch/app/article/oeuvre-1922-09-22-a-i0093) | L'ASSEMBLÉE DE LA SOCIÉTÉ DES NATIONS s'occupe de la protection des mi[...] | 1922-09-22 | oeuvre; oeuvre-1922-09-15-a-i0030 (https://impresso-project.ch/app/article/oeuvre-1922-09-15-a-i0030) | A GENÈVE, PENDANT L'ENTR'ACTE : Le projet de Lord Robert Cecil a fait [...] | 1922-09-15 | oeuvre; LSE-1922-10-11-a-i0002 (https://impresso-project.ch/app/article/LSE-1922-10-11-a-i0002) | EN EUROPE CENTRALE Aux Chambres féd | 1922-10-11 | LSE; GDL-1922-08-03-a-i0012 (https://impresso-project.ch/app/article/GDL-1922-08-03-a-i0012) | Sa fia. Ni | 1922-08-03 | GDL; NZZ-1922-09-23-a-i0002 (https://impresso-project.ch/app/article/NZZ-1922-09-23-a-i0002) | [Sans titre] | 1922-09-23 | NZZ; LSE-1922-09-15-a-i0001 (https://impresso-project.ch/app/article/LSE-1922-09-15-a-i0001) | Quotidien socialiste |OT~Citoyens suisses, ne vous laissez pas museler[...] | 1922-09-15 | LSE; GDL-1922-09-14-a-i0011 (https://impresso-project.ch/app/article/GDL-1922-09-14-a-i0011) | 9B ÊEB NB | 1922-09-14 | GDL; NZZ-1922-09-29-c-i0002 (https://impresso-project.ch/app/article/NZZ-1922-09-29-c-i0002) | [Sans titre] | 1922-09-29 | NZZ; LSE-1922-10-10-a-i0001 (https://impresso-project.ch/app/article/LSE-1922-10-10-a-i0001) | La Sentinelle Quotidien socialiste Lecteurs, achetez de préférence l’Â[...] | 1922-10-10 | LSE; NZZ-1922-09-21-a-i0010 (https://impresso-project.ch/app/article/NZZ-1922-09-21-a-i0010) | [Sans titre] | 1922-09-21 | NZZ; NZZ-1922-09-21-a-i0002 (https://impresso-project.ch/app/article/NZZ-1922-09-21-a-i0002) | [Sans titre] | 1922-09-21 | NZZ; NZZ-1922-09-15-b-i0001 (https://impresso-project.ch/app/article/NZZ-1922-09-15-b-i0001) | [Sans titre] | 1922-09-15 | NZZ; NZZ-1922-09-11-b-i0014 (https://impresso-project.ch/app/article/NZZ-1922-09-11-b-i0014) | [Sans titre] | 1922-09-11 | NZZ; NZZ-1922-09-26-c-i0002 (https://impresso-project.ch/app/article/NZZ-1922-09-26-c-i0002) | [Sans titre] | 1922-09-26 | NZZ; LLE-1922-09-07-a-i0006 (https://impresso-project.ch/app/article/LLE-1922-09-07-a-i0006) | Société des nations | 1922-09-07 | LLE</t>
+  </si>
+  <si>
+    <t>JDG-1922-08-21-a-i0029 (https://impresso-project.ch/app/article/JDG-1922-08-21-a-i0029) | CARNET DU JOUR | 1922-08-21 | JDG; LES-1922-08-19-a-i0010 (https://impresso-project.ch/app/article/LES-1922-08-19-a-i0010) | Le Bureau International raueaiion | 1922-08-19 | LES; GDL-1922-08-06-a-i0011 (https://impresso-project.ch/app/article/GDL-1922-08-06-a-i0011) | S&amp;gt; dL ra | 1922-08-06 | GDL; JDG-1922-08-23-a-i0044 (https://impresso-project.ch/app/article/JDG-1922-08-23-a-i0044) | [Sans titre] | 1922-08-23 | JDG; JDG-1922-08-20-a-i0054 (https://impresso-project.ch/app/article/JDG-1922-08-20-a-i0054) | CARNET DU JOUR | 1922-08-20 | JDG; JDG-1922-09-16-a-i0040 (https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0040) | [Sans titre] | 1922-09-16 | JDG; JDG-1922-09-17-a-i0054 (https://impresso-project.ch/app/article/JDG-1922-09-17-a-i0054) | ÛEiÈWE | 1922-09-17 | JDG; JDG-1922-08-15-a-i0041 (https://impresso-project.ch/app/article/JDG-1922-08-15-a-i0041) | CARNET DU JOUR | 1922-08-15 | JDG; JDG-1922-08-19-a-i0045 (https://impresso-project.ch/app/article/JDG-1922-08-19-a-i0045) | GENÈVE | 1922-08-19 | JDG; JDG-1922-08-11-a-i0042 (https://impresso-project.ch/app/article/JDG-1922-08-11-a-i0042) | GENÈV E | 1922-08-11 | JDG; JDG-1922-08-05-a-i0017 (https://impresso-project.ch/app/article/JDG-1922-08-05-a-i0017) | Société des dations | 1922-08-05 | JDG; JDG-1922-08-11-a-i0043 (https://impresso-project.ch/app/article/JDG-1922-08-11-a-i0043) | CARNET DU JOUR | 1922-08-11 | JDG; JDG-1922-08-13-a-i0043 (https://impresso-project.ch/app/article/JDG-1922-08-13-a-i0043) | GENÈVE | 1922-08-13 | JDG; JDG-1922-08-19-a-i0048 (https://impresso-project.ch/app/article/JDG-1922-08-19-a-i0048) | CARNET DU JOUR | 1922-08-19 | JDG; NZZ-1922-08-13-d-i0001 (https://impresso-project.ch/app/article/NZZ-1922-08-13-d-i0001) | [Sans titre] | 1922-08-13 | NZZ</t>
+  </si>
+  <si>
+    <t>indeplux-1922-10-16-a-i0001 (https://impresso-project.ch/app/article/indeplux-1922-10-16-a-i0001) | Billet extérieur | 1922-10-16 | indeplux; indeplux-1922-09-04-a-i0001 (https://impresso-project.ch/app/article/indeplux-1922-09-04-a-i0001) | Billet extérieur | 1922-09-04 | indeplux; indeplux-1922-09-18-a-i0001 (https://impresso-project.ch/app/article/indeplux-1922-09-18-a-i0001) | Billet extérieur | 1922-09-18 | indeplux; indeplux-1922-10-30-a-i0001 (https://impresso-project.ch/app/article/indeplux-1922-10-30-a-i0001) | Billet extérieur | 1922-10-30 | indeplux; indeplux-1922-08-16-a-i0001 (https://impresso-project.ch/app/article/indeplux-1922-08-16-a-i0001) | Billet extérieur | 1922-08-16 | indeplux; indeplux-1922-10-23-a-i0001 (https://impresso-project.ch/app/article/indeplux-1922-10-23-a-i0001) | Billet extérieur | 1922-10-23 | indeplux; indeplux-1922-10-09-a-i0001 (https://impresso-project.ch/app/article/indeplux-1922-10-09-a-i0001) | Billet extérieur | 1922-10-09 | indeplux; indeplux-1922-08-21-a-i0001 (https://impresso-project.ch/app/article/indeplux-1922-08-21-a-i0001) | Billet extérieur | 1922-08-21 | indeplux; indeplux-1922-09-13-a-i0001 (https://impresso-project.ch/app/article/indeplux-1922-09-13-a-i0001) | Billet extérieur | 1922-09-13 | indeplux; indeplux-1922-08-28-a-i0001 (https://impresso-project.ch/app/article/indeplux-1922-08-28-a-i0001) | Billet extérieur | 1922-08-28 | indeplux; indeplux-1922-09-25-a-i0001 (https://impresso-project.ch/app/article/indeplux-1922-09-25-a-i0001) | Billet extérieur | 1922-09-25 | indeplux; indeplux-1922-08-08-a-i0001 (https://impresso-project.ch/app/article/indeplux-1922-08-08-a-i0001) | Billet extérieur | 1922-08-08 | indeplux; EXP-1922-09-02-a-i0094 (https://impresso-project.ch/app/article/EXP-1922-09-02-a-i0094) | POLITIQUE , | 1922-09-02 | EXP</t>
+  </si>
+  <si>
+    <t>GDL-1922-08-21-a-i0020 (https://impresso-project.ch/app/article/GDL-1922-08-21-a-i0020) | 9B CB Sa | 1922-08-21 | GDL; indeplux-1922-08-23-a-i0019 (https://impresso-project.ch/app/article/indeplux-1922-08-23-a-i0019) | M. Léon Bérard et l’Espéranto | 1922-08-23 | indeplux; lepetitparisien-1922-08-24-a-i0070 (https://impresso-project.ch/app/article/lepetitparisien-1922-08-24-a-i0070) | L'ESPÉRANTO | 1922-08-24 | lepetitparisien; NZZ-1922-09-25-a-i0005 (https://impresso-project.ch/app/article/NZZ-1922-09-25-a-i0005) | [Sans titre] | 1922-09-25 | NZZ</t>
+  </si>
+  <si>
+    <t>EXP-1922-08-24-a-i0049 (https://impresso-project.ch/app/article/EXP-1922-08-24-a-i0049) | POLITIQUE | 1922-08-24 | EXP; JDG-1922-08-23-a-i0107 (https://impresso-project.ch/app/article/JDG-1922-08-23-a-i0107) | Société des Nations | 1922-08-23 | JDG</t>
+  </si>
+  <si>
+    <t>EXP-1922-09-13-a-i0069 (https://impresso-project.ch/app/article/EXP-1922-09-13-a-i0069) | POLITIQUE Société des nations | 1922-09-13 | EXP; JDG-1922-09-13-a-i0020 (https://impresso-project.ch/app/article/JDG-1922-09-13-a-i0020) | Société des nations | 1922-09-13 | JDG; oecaen-1922-09-20-a-i0031 (https://impresso-project.ch/app/article/oecaen-1922-09-20-a-i0031) | &lt; LA FXiBCHB | 1922-09-20 | oecaen; oeuvre-1922-09-19-a-i0026 (https://impresso-project.ch/app/article/oeuvre-1922-09-19-a-i0026) | LA DIXIÈME ASSAMBLEE PLÊNIÈRE | 1922-09-19 | oeuvre</t>
+  </si>
+  <si>
+    <t>oeuvre-1922-08-05-a-i0034 (https://impresso-project.ch/app/article/oeuvre-1922-08-05-a-i0034) | L'Amérique et la Société des Nations | 1922-08-05 | oeuvre; GDL-1922-08-17-a-i0074 (https://impresso-project.ch/app/article/GDL-1922-08-17-a-i0074) | [Sans titre] | 1922-08-17 | GDL; JDG-1922-08-17-a-i0083 (https://impresso-project.ch/app/article/JDG-1922-08-17-a-i0083) | Société des Nations | 1922-08-17 | JDG; lematin-1922-09-19-a-i0039 (https://impresso-project.ch/app/article/lematin-1922-09-19-a-i0039) | Les secours aux réfugiés de Smyrne | 1922-09-19 | lematin; JDG-1922-09-10-a-i0016 (https://impresso-project.ch/app/article/JDG-1922-09-10-a-i0016) | DISCUSSIO N GENERAL E SU R L E RAPPOR T D U CONSEI L | 1922-09-10 | JDG; JDG-1922-10-27-a-i0044 (https://impresso-project.ch/app/article/JDG-1922-10-27-a-i0044) | IV me C©nféreisce du îravai | 1922-10-27 | JDG; JDG-1922-09-19-a-i0090 (https://impresso-project.ch/app/article/JDG-1922-09-19-a-i0090) | S me EDITION Société des nations | 1922-09-19 | JDG; EXP-1922-08-18-a-i0035 (https://impresso-project.ch/app/article/EXP-1922-08-18-a-i0035) | POLITIQUE | 1922-08-18 | EXP; JDG-1922-10-02-a-i0020 (https://impresso-project.ch/app/article/JDG-1922-10-02-a-i0020) | Société des nations | 1922-10-02 | JDG; GDL-1922-09-04-a-i0071 (https://impresso-project.ch/app/article/GDL-1922-09-04-a-i0071) | Sa da | 1922-09-04 | GDL; legaulois-1922-10-03-a-i0004 (https://impresso-project.ch/app/article/legaulois-1922-10-03-a-i0004) | DANS LE MONDE OFFICIEL | 1922-10-03 | legaulois; EXP-1922-09-04-a-i0056 (https://impresso-project.ch/app/article/EXP-1922-09-04-a-i0056) | APOLITIQUE | 1922-09-04 | EXP; GDL-1922-09-29-a-i0010 (https://impresso-project.ch/app/article/GDL-1922-09-29-a-i0010) | L'Azerbaïdjan et la S. d. | 1922-09-29 | GDL; NZZ-1922-09-19-a-i0002 (https://impresso-project.ch/app/article/NZZ-1922-09-19-a-i0002) | [Sans titre] | 1922-09-19 | NZZ; LLE-1922-09-05-a-i0002 (https://impresso-project.ch/app/article/LLE-1922-09-05-a-i0002) | La troisième assemblée de la Société des... | 1922-09-05 | LLE; luxwort-1922-09-05-a-i0058 (https://impresso-project.ch/app/article/luxwort-1922-09-05-a-i0058) | Die 3. Völkerbundsversammlung in Genf. | 1922-09-05 | luxwort; NZZ-1922-09-03-a-i0002 (https://impresso-project.ch/app/article/NZZ-1922-09-03-a-i0002) | [Sans titre] | 1922-09-03 | NZZ; FZG-1922-08-18-a-i0038 (https://impresso-project.ch/app/article/FZG-1922-08-18-a-i0038) | «danken die schwerste «Niederlage. «Gin ... | 1922-08-18 | FZG; NZZ-1922-10-23-d-i0001 (https://impresso-project.ch/app/article/NZZ-1922-10-23-d-i0001) | [Sans titre] | 1922-10-23 | NZZ; FZG-1922-10-24-a-i0014 (https://impresso-project.ch/app/article/FZG-1922-10-24-a-i0014) | mmmm W&gt;/AL- rMsh*.*.*» A. •*&amp; Jts-**i | 1922-10-24 | FZG; NZZ-1922-09-03-a-i0009 (https://impresso-project.ch/app/article/NZZ-1922-09-03-a-i0009) | [Sans titre] | 1922-09-03 | NZZ; FZG-1922-09-04-a-i0015 (https://impresso-project.ch/app/article/FZG-1922-09-04-a-i0015) | • Neueste Meldunam # | 1922-09-04 | FZG; FZG-1922-09-02-a-i0022 (https://impresso-project.ch/app/article/FZG-1922-09-02-a-i0022) | Jum griechisch«türkische Konflikt. Adana... | 1922-09-02 | FZG</t>
+  </si>
+  <si>
+    <t>indeplux-1922-09-22-a-i0018 (https://impresso-project.ch/app/article/indeplux-1922-09-22-a-i0018) | Société des Nations Une note exprimant les vœux de la France sera prés[...] | 1922-09-22 | indeplux; legaulois-1922-09-12-a-i0025 (https://impresso-project.ch/app/article/legaulois-1922-09-12-a-i0025) | Réponse de lord Robert Cecil | 1922-09-12 | legaulois; oeuvre-1922-09-14-a-i0036 (https://impresso-project.ch/app/article/oeuvre-1922-09-14-a-i0036) | M. LLOYD GEORGE VIENDRA-T-IL A GENÈVE ? | 1922-09-14 | oeuvre; EXP-1922-09-08-a-i0066 (https://impresso-project.ch/app/article/EXP-1922-09-08-a-i0066) | POLITIQUE Société des Nations | 1922-09-08 | EXP; oeuvre-1922-10-08-a-i0033 (https://impresso-project.ch/app/article/oeuvre-1922-10-08-a-i0033) | Le Dr Nansen organise une mission purement britannique | 1922-10-08 | oeuvre; oeuvre-1922-09-20-a-i0027 (https://impresso-project.ch/app/article/oeuvre-1922-09-20-a-i0027) | LE PROBLÈME DES RÉPARATIONS | 1922-09-20 | oeuvre; legaulois-1922-09-23-a-i0032 (https://impresso-project.ch/app/article/legaulois-1922-09-23-a-i0032) | A LA SOCIÉTÉ DES MATIONS | 1922-09-23 | legaulois; legaulois-1922-09-01-a-i0016 (https://impresso-project.ch/app/article/legaulois-1922-09-01-a-i0016) | Dernière Heure Â la Société des Nations | 1922-09-01 | legaulois; indeplux-1922-09-14-a-i0046 (https://impresso-project.ch/app/article/indeplux-1922-09-14-a-i0046) | Un accord intervient entre lord Robert ( ecil et M. de Jouvenel au suj[...] | 1922-09-14 | indeplux; indeplux-1922-09-23-a-i0030 (https://impresso-project.ch/app/article/indeplux-1922-09-23-a-i0030) | Le point de vue français sur le désarmement | 1922-09-23 | indeplux; lematin-1922-09-13-a-i0057 (https://impresso-project.ch/app/article/lematin-1922-09-13-a-i0057) | La commission adopté le projet de lord Robert Cecil sur le désarmement | 1922-09-13 | lematin; JDG-1922-09-09-a-i0010 (https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0010) | LÀ SITUATION | 1922-09-09 | JDG; JDG-1922-09-08-a-i0001 (https://impresso-project.ch/app/article/JDG-1922-09-08-a-i0001) | BULLETIN | 1922-09-08 | JDG; legaulois-1922-09-19-a-i0014 (https://impresso-project.ch/app/article/legaulois-1922-09-19-a-i0014) | A la Société des Nations | 1922-09-19 | legaulois; legaulois-1922-09-14-a-i0023 (https://impresso-project.ch/app/article/legaulois-1922-09-14-a-i0023) | Vers un pacte de garantie | 1922-09-14 | legaulois; legaulois-1922-09-07-a-i0045 (https://impresso-project.ch/app/article/legaulois-1922-09-07-a-i0045) | Le Chancelier d'Autriche expose la détresse de son pays | 1922-09-07 | legaulois; lematin-1922-09-23-a-i0037 (https://impresso-project.ch/app/article/lematin-1922-09-23-a-i0037) | LaS.D.N. s'occupe du conflit gréco-turc | 1922-09-23 | lematin; lepetitparisien-1922-09-12-a-i0032 (https://impresso-project.ch/app/article/lepetitparisien-1922-09-12-a-i0032) | A L'ASSEMBLÉE de la Société des Nations | 1922-09-12 | lepetitparisien; JDG-1922-09-09-a-i0017 (https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0017) | M. Sciai oj? | 1922-09-09 | JDG; oeuvre-1922-09-23-a-i0039 (https://impresso-project.ch/app/article/oeuvre-1922-09-23-a-i0039) | La question d'Orient | 1922-09-23 | oeuvre; lematin-1922-09-16-a-i0031 (https://impresso-project.ch/app/article/lematin-1922-09-16-a-i0031) | La réduction des armements doit dépendre des garanties données par le [...] | 1922-09-16 | lematin; EXP-1922-09-18-a-i0049 (https://impresso-project.ch/app/article/EXP-1922-09-18-a-i0049) | 1POLITIQUE&amp;gt;£.i | 1922-09-18 | EXP; IMP-1922-09-12-a-i0002 (https://impresso-project.ch/app/article/IMP-1922-09-12-a-i0002) | ba Semaine internationale | 1922-09-12 | IMP; JDG-1922-09-09-a-i0008 (https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0008) | t&amp;UrcS | 1922-09-09 | JDG; EXP-1922-10-03-a-i0092 (https://impresso-project.ch/app/article/EXP-1922-10-03-a-i0092) | Chronique parlementaire | 1922-10-03 | EXP; indeplux-1922-09-23-a-i0051 (https://impresso-project.ch/app/article/indeplux-1922-09-23-a-i0051) | DERNIÈRE HEURE | 1922-09-23 | indeplux; IMP-1922-10-03-a-i0001 (https://impresso-project.ch/app/article/IMP-1922-10-03-a-i0001) | L&amp;gt;a Semaine internationale | 1922-10-03 | IMP; lematin-1922-09-17-a-i0038 (https://impresso-project.ch/app/article/lematin-1922-09-17-a-i0038) | Un émouvant débat entre le délégué français et le délégué anglais | 1922-09-17 | lematin; oeuvre-1922-10-12-a-i0008 (https://impresso-project.ch/app/article/oeuvre-1922-10-12-a-i0008) | M. Lloyd George prépare contre ses détracteurs une grande bataille | 1922-10-12 | oeuvre; JDG-1922-09-01-a-i0001 (https://impresso-project.ch/app/article/JDG-1922-09-01-a-i0001) | [Sans titre] | 1922-09-01 | JDG; JDG-1922-09-28-a-i0001 (https://impresso-project.ch/app/article/JDG-1922-09-28-a-i0001) | [Sans titre] | 1922-09-28 | JDG; EXP-1922-08-23-a-i0043 (https://impresso-project.ch/app/article/EXP-1922-08-23-a-i0043) | POLITIQUE | 1922-08-23 | EXP; legaulois-1922-09-17-a-i0019 (https://impresso-project.ch/app/article/legaulois-1922-09-17-a-i0019) | Dernière A LA SOCIÉTÉ DES NATIONS | 1922-09-17 | legaulois; legaulois-1922-09-18-a-i0018 (https://impresso-project.ch/app/article/legaulois-1922-09-18-a-i0018) | Dernière Heure AU SOCIÉTÉ DES MATIONS | 1922-09-18 | legaulois; GDL-1922-09-21-a-i0061 (https://impresso-project.ch/app/article/GDL-1922-09-21-a-i0061) | La troisième session de la S. d. N. | 1922-09-21 | GDL; GDL-1922-09-14-a-i0059 (https://impresso-project.ch/app/article/GDL-1922-09-14-a-i0059) | Chronique de la S. d.N | 1922-09-14 | GDL; EXP-1922-10-06-a-i0093 (https://impresso-project.ch/app/article/EXP-1922-10-06-a-i0093) | Après la session | 1922-10-06 | EXP; legaulois-1922-09-08-a-i0034 (https://impresso-project.ch/app/article/legaulois-1922-09-08-a-i0034) | A LA SOCIÉTÉ DES KATIONS | 1922-09-08 | legaulois; legaulois-1922-09-12-a-i0024 (https://impresso-project.ch/app/article/legaulois-1922-09-12-a-i0024) | A LA SOCIÉTÉ DES NATIONS | 1922-09-12 | legaulois; lematin-1922-09-13-a-i0077 (https://impresso-project.ch/app/article/lematin-1922-09-13-a-i0077) | LA PROCHAINE ARRIVÉE DE M. LLOYD GEORGE A GENÈVE | 1922-09-13 | lematin; JDG-1922-09-15-a-i0090 (https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0090) | Le plan Cecil et la doctrine d e Monroë | 1922-09-15 | JDG; EXP-1922-09-13-a-i0043 (https://impresso-project.ch/app/article/EXP-1922-09-13-a-i0043) | POLITIQUE Société des ffati _ * __§ | 1922-09-13 | EXP; GDL-1922-08-23-a-i0012 (https://impresso-project.ch/app/article/GDL-1922-08-23-a-i0012) | S. | 1922-08-23 | GDL; JDG-1922-09-15-a-i0006 (https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0006) | BULLETIN | 1922-09-15 | JDG; JDG-1922-10-05-a-i0006 (https://impresso-project.ch/app/article/JDG-1922-10-05-a-i0006) | Chronique parlementaire | 1922-10-05 | JDG; JDG-1922-09-22-a-i0010 (https://impresso-project.ch/app/article/JDG-1922-09-22-a-i0010) | [Sans titre] | 1922-09-22 | JDG; EXP-1922-09-13-a-i0074 (https://impresso-project.ch/app/article/EXP-1922-09-13-a-i0074) | DERNIERES REPÊCHES | 1922-09-13 | EXP; lematin-1922-09-15-a-i0053 (https://impresso-project.ch/app/article/lematin-1922-09-15-a-i0053) | Le délégué français propose, comme première mesure de réduire les dépe[...] | 1922-09-15 | lematin; EXP-1922-09-22-a-i0051 (https://impresso-project.ch/app/article/EXP-1922-09-22-a-i0051) | Sodttè des nations | 1922-09-22 | EXP; IMP-1922-09-28-a-i0029 (https://impresso-project.ch/app/article/IMP-1922-09-28-a-i0029) | Ledésarmement devant l'Assemblée de Genève | 1922-09-28 | IMP; legaulois-1922-09-28-a-i0054 (https://impresso-project.ch/app/article/legaulois-1922-09-28-a-i0054) | h la Société des gâtions | 1922-09-28 | legaulois; oeuvre-1922-09-20-a-i0026 (https://impresso-project.ch/app/article/oeuvre-1922-09-20-a-i0026) | LE PACTE DE GARANTIE | 1922-09-20 | oeuvre; JDG-1922-09-14-a-i0020 (https://impresso-project.ch/app/article/JDG-1922-09-14-a-i0020) | L'attitude de l'Argentine | 1922-09-14 | JDG; JDG-1922-09-20-a-i0090 (https://impresso-project.ch/app/article/JDG-1922-09-20-a-i0090) | Société des nations | 1922-09-20 | JDG; JDG-1922-09-23-a-i0002 (https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0002) | GENEVE, 22 septembre 1922 TJX.LETIN | 1922-09-23 | JDG; JDG-1922-09-16-a-i0073 (https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0073) | 2me EDITION....III Société des nations | 1922-09-16 | JDG; legaulois-1922-09-20-a-i0025 (https://impresso-project.ch/app/article/legaulois-1922-09-20-a-i0025) | A LA SOCIÉTÉ DES NATIONS | 1922-09-20 | legaulois; GDL-1922-09-09-a-i0004 (https://impresso-project.ch/app/article/GDL-1922-09-09-a-i0004) | La troisième session de la S. d. N. | 1922-09-09 | GDL; lematin-1922-09-14-a-i0050 (https://impresso-project.ch/app/article/lematin-1922-09-14-a-i0050) | Le pacte de garantie n'affectera aucunement les traités de paix | 1922-09-14 | lematin; JDG-1922-09-17-a-i0113 (https://impresso-project.ch/app/article/JDG-1922-09-17-a-i0113) | gme EDITION ^•.IH.,.1.1.1— i •• - ...M..,,.,— •• '- • IM.-H..MI.III So[...] | 1922-09-17 | JDG; lepetitparisien-1922-09-03-a-i0039 (https://impresso-project.ch/app/article/lepetitparisien-1922-09-03-a-i0039) | La troisième assemblée de la Société des nations | 1922-09-03 | lepetitparisien; indeplux-1922-09-14-a-i0043 (https://impresso-project.ch/app/article/indeplux-1922-09-14-a-i0043) | La Commission du Désarmement discute la proposition de pacte de garant[...] | 1922-09-14 | indeplux; indeplux-1922-09-28-a-i0039 (https://impresso-project.ch/app/article/indeplux-1922-09-28-a-i0039) | Société des Nations La discussion sur la réduction des armements se po[...] | 1922-09-28 | indeplux; lematin-1922-09-27-a-i0030 (https://impresso-project.ch/app/article/lematin-1922-09-27-a-i0030) | Quand donc l'humanité "* , » nous apportant le pacte de garantie, dira[...] | 1922-09-27 | lematin; oecaen-1922-09-19-a-i0034 (https://impresso-project.ch/app/article/oecaen-1922-09-19-a-i0034) | UN NOUVEAU TEXTE | 1922-09-19 | oecaen; oecaen-1922-09-27-a-i0006 (https://impresso-project.ch/app/article/oecaen-1922-09-27-a-i0006) | Les travaux de la Commission du Désarmement devant l'Assemblée | 1922-09-27 | oecaen; JDG-1922-09-13-a-i0002 (https://impresso-project.ch/app/article/JDG-1922-09-13-a-i0002) | fc&amp;S | 1922-09-13 | JDG; GDL-1922-09-27-a-i0004 (https://impresso-project.ch/app/article/GDL-1922-09-27-a-i0004) | La troisième session aelaJjLd.ll. Dix-septième séance plénière | 1922-09-27 | GDL; legaulois-1922-08-26-a-i0038 (https://impresso-project.ch/app/article/legaulois-1922-08-26-a-i0038) | Revue de la Presse | 1922-08-26 | legaulois; EXP-1922-09-06-a-i0059 (https://impresso-project.ch/app/article/EXP-1922-09-06-a-i0059) | POLITIQUE Société cS@s Nattons | 1922-09-06 | EXP; lepetitparisien-1922-09-09-a-i0056 (https://impresso-project.ch/app/article/lepetitparisien-1922-09-09-a-i0056) | CE QUE LA FRANCE A FAIT pour diminuer ses armements | 1922-09-09 | lepetitparisien; indeplux-1922-08-31-a-i0027 (https://impresso-project.ch/app/article/indeplux-1922-08-31-a-i0027) | Une proposition de lord Robert Cecil au sujet du désarmement | 1922-08-31 | indeplux; oeuvre-1922-10-25-a-i0001 (https://impresso-project.ch/app/article/oeuvre-1922-10-25-a-i0001) | POUR QUE L'ENTENTE REDEVIENNE CORDIALE : Définissons nos « buts de pai[...] | 1922-10-25 | oeuvre; oeuvre-1922-09-23-a-i0038 (https://impresso-project.ch/app/article/oeuvre-1922-09-23-a-i0038) | Un foyer national pour les Arméniens | 1922-09-23 | oeuvre; JDG-1922-09-09-a-i0015 (https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0015) | Assemblée de fa Société des nations | 1922-09-09 | JDG; JDG-1922-09-23-a-i0099 (https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0099) | TROISIEME EDITION La guerre en Asie Mineure et le problème du proche O[...] | 1922-09-23 | JDG; JDG-1922-09-21-a-i0027 (https://impresso-project.ch/app/article/JDG-1922-09-21-a-i0027) | Dans les Commissions | 1922-09-21 | JDG; legaulois-1922-09-13-a-i0021 (https://impresso-project.ch/app/article/legaulois-1922-09-13-a-i0021) | A LA SOCIÉTÉ DES NATIONS | 1922-09-13 | legaulois; JDG-1922-09-27-a-i0005 (https://impresso-project.ch/app/article/JDG-1922-09-27-a-i0005) | Assemblée de la Société des nations Séance plénière d | 1922-09-27 | JDG; EXP-1922-10-28-a-i0069 (https://impresso-project.ch/app/article/EXP-1922-10-28-a-i0069) | COÏÏREÎER FRANÇAIS | 1922-10-28 | EXP; IMP-1922-09-04-a-i0003 (https://impresso-project.ch/app/article/IMP-1922-09-04-a-i0003) | Lettre de Genève | 1922-09-04 | IMP; lematin-1922-09-18-a-i0089 (https://impresso-project.ch/app/article/lematin-1922-09-18-a-i0089) | L'opinion de lord Robert Ceci! sur l'admission du Reich dans la S. D. [...] | 1922-09-18 | lematin; oecaen-1922-09-18-a-i0016 (https://impresso-project.ch/app/article/oecaen-1922-09-18-a-i0016) | Lord Robert Cecfl est partisan de l'admission de l'Allemagne à la SM. | 1922-09-18 | oecaen; indeplux-1922-09-06-a-i0012 (https://impresso-project.ch/app/article/indeplux-1922-09-06-a-i0012) | L’Assemblée de la S. d. N. | 1922-09-06 | indeplux; lematin-1922-09-01-a-i0002 (https://impresso-project.ch/app/article/lematin-1922-09-01-a-i0002) | M. Lloyd George ira-t-il à Genève? | 1922-09-01 | lematin; oeuvre-1922-09-21-a-i0038 (https://impresso-project.ch/app/article/oeuvre-1922-09-21-a-i0038) | Comment la Belgique négociera les bons allemands | 1922-09-21 | oeuvre; lepetitparisien-1922-10-01-a-i0025 (https://impresso-project.ch/app/article/lepetitparisien-1922-10-01-a-i0025) | LA SOCIÉTÉ DES NATIONS a clos hier ses travaux | 1922-10-01 | lepetitparisien; indeplux-1922-09-04-a-i0008 (https://impresso-project.ch/app/article/indeplux-1922-09-04-a-i0008) | La Commission approuve le projet de lord Robert Cecil sur le desarmeme[...] | 1922-09-04 | indeplux; legaulois-1922-09-16-a-i0021 (https://impresso-project.ch/app/article/legaulois-1922-09-16-a-i0021) | SHAKESPEARE Fils de la Reine Elisabeth | 1922-09-16 | legaulois; JDG-1922-09-23-a-i0004 (https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0004) | L'Allemagne et ia Société des nations | 1922-09-23 | JDG; IMP-1922-09-26-a-i0002 (https://impresso-project.ch/app/article/IMP-1922-09-26-a-i0002) | ba Semaine internationale | 1922-09-26 | IMP; legaulois-1922-08-04-a-i0062 (https://impresso-project.ch/app/article/legaulois-1922-08-04-a-i0062) | Le débat à la Chambre des Communes | 1922-08-04 | legaulois; GDL-1922-09-08-a-i0006 (https://impresso-project.ch/app/article/GDL-1922-09-08-a-i0006) | La troisième session de la S. d. N. | 1922-09-08 | GDL; EXP-1922-09-14-a-i0094 (https://impresso-project.ch/app/article/EXP-1922-09-14-a-i0094) | \. POLITIQUE Société des nations | 1922-09-14 | EXP; indeplux-1922-09-07-a-i0028 (https://impresso-project.ch/app/article/indeplux-1922-09-07-a-i0028) | Un discours de lord Robert Cecil | 1922-09-07 | indeplux; legaulois-1922-09-15-a-i0026 (https://impresso-project.ch/app/article/legaulois-1922-09-15-a-i0026) | Les Journaux du matin | 1922-09-15 | legaulois; legaulois-1922-09-21-a-i0035 (https://impresso-project.ch/app/article/legaulois-1922-09-21-a-i0035) | Les Journaux du matin | 1922-09-21 | legaulois; GDL-1922-09-18-a-i0060 (https://impresso-project.ch/app/article/GDL-1922-09-18-a-i0060) | 9a fia Ni | 1922-09-18 | GDL; lematin-1922-09-20-a-i0041 (https://impresso-project.ch/app/article/lematin-1922-09-20-a-i0041) | M. de Jouvenel fait, an nom de la délégation française ' I' .. v" une [...] | 1922-09-20 | lematin; lematin-1922-10-20-a-i0051 (https://impresso-project.ch/app/article/lematin-1922-10-20-a-i0051) | LES GRANDS RETOURS | 1922-10-20 | lematin; IMP-1922-09-09-a-i0026 (https://impresso-project.ch/app/article/IMP-1922-09-09-a-i0026) | Lettre de Genève | 1922-09-09 | IMP; IMP-1922-09-20-a-i0001 (https://impresso-project.ch/app/article/IMP-1922-09-20-a-i0001) | ba Semaine internationale | 1922-09-20 | IMP; JDG-1922-09-09-a-i0027 (https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0027) | En marge de l'Assemblée Réceptio n officiell e | 1922-09-09 | JDG; JDG-1922-09-15-a-i0083 (https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0083) | La guerre en Anatolie et le problème du proche Orient | 1922-09-15 | JDG; lematin-1922-09-06-a-i0071 (https://impresso-project.ch/app/article/lematin-1922-09-06-a-i0071) | L'assemblée de Genève nomme ses commissions | 1922-09-06 | lematin</t>
+  </si>
+  <si>
+    <t>legaulois-1922-10-28-a-i0013 (https://impresso-project.ch/app/article/legaulois-1922-10-28-a-i0013) | NÉCROLOGIE | 1922-10-28 | legaulois; oecaen-1922-09-26-a-i0049 (https://impresso-project.ch/app/article/oecaen-1922-09-26-a-i0049) | TRIBUNAL CORRECTIONNEL | 1922-09-26 | oecaen; lepetitparisien-1922-08-22-a-i0053 (https://impresso-project.ch/app/article/lepetitparisien-1922-08-22-a-i0053) | LECONORÈS UNIVERSEL D'ESPERANTO | 1922-08-22 | lepetitparisien; lematin-1922-08-08-a-i0074 (https://impresso-project.ch/app/article/lematin-1922-08-08-a-i0074) | NOUVELLES EN TROIS LIGNES | 1922-08-08 | lematin; oecaen-1922-08-06-a-i0080 (https://impresso-project.ch/app/article/oecaen-1922-08-06-a-i0080) | I !MJbv3 | 1922-08-06 | oecaen</t>
+  </si>
+  <si>
+    <t>indeplux-1922-08-03-a-i0038 (https://impresso-project.ch/app/article/indeplux-1922-08-03-a-i0038) | ITALIE La constitution définitive du ministère Facta | 1922-08-03 | indeplux; GDL-1922-08-02-a-i0013 (https://impresso-project.ch/app/article/GDL-1922-08-02-a-i0013) | Les consultations de M. Facta | 1922-08-02 | GDL; luxwort-1922-08-03-a-i0001 (https://impresso-project.ch/app/article/luxwort-1922-08-03-a-i0001) | Zur Kabinettsumbildung in Italien. | 1922-08-03 | luxwort; NZZ-1922-08-01-b-i0006 (https://impresso-project.ch/app/article/NZZ-1922-08-01-b-i0006) | [Sans titre] | 1922-08-01 | NZZ; NZZ-1922-10-18-a-i0002 (https://impresso-project.ch/app/article/NZZ-1922-10-18-a-i0002) | [Sans titre] | 1922-10-18 | NZZ</t>
+  </si>
+  <si>
+    <t>JDG-1922-10-09-a-i0021 (https://impresso-project.ch/app/article/JDG-1922-10-09-a-i0021) | Société des Nations | 1922-10-09 | JDG</t>
+  </si>
+  <si>
+    <t>LES-1922-08-05-a-i0020 (https://impresso-project.ch/app/article/LES-1922-08-05-a-i0020) | Encore si cette revue dépassait par la r... | 1922-08-05 | LES; JDG-1922-09-16-a-i0036 (https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0036) | A propos du droit d'auteur | 1922-09-16 | JDG; LCE-1922-09-11-a-i0010 (https://impresso-project.ch/app/article/LCE-1922-09-11-a-i0010) | En Suisse Cordages en loysoeoresTravai. Soi C. Kissimg. cordier, Ullle[...] | 1922-09-11 | LCE; GDL-1922-09-08-a-i0018 (https://impresso-project.ch/app/article/GDL-1922-09-08-a-i0018) | CONFÉDÉRATION | 1922-09-08 | GDL; NZZ-1922-09-11-b-i0021 (https://impresso-project.ch/app/article/NZZ-1922-09-11-b-i0021) | [Sans titre] | 1922-09-11 | NZZ; NZZ-1922-10-05-a-i0001 (https://impresso-project.ch/app/article/NZZ-1922-10-05-a-i0001) | [Sans titre] | 1922-10-05 | NZZ; LLE-1922-09-04-a-i0019 (https://impresso-project.ch/app/article/LLE-1922-09-04-a-i0019) | Les réformes constitutionnelles au Tessi... | 1922-09-04 | LLE; FZG-1922-08-26-a-i0017 (https://impresso-project.ch/app/article/FZG-1922-08-26-a-i0017) | Schweiz | 1922-08-26 | FZG</t>
+  </si>
+  <si>
+    <t>JDG-1922-08-26-a-i0095 (https://impresso-project.ch/app/article/JDG-1922-08-26-a-i0095) | Nos hôtes | 1922-08-26 | JDG; lematin-1922-08-06-a-i0076 (https://impresso-project.ch/app/article/lematin-1922-08-06-a-i0076) | Le président de la Confédération helvétique h la Société des nations | 1922-08-06 | lematin; lematin-1922-09-14-a-i0051 (https://impresso-project.ch/app/article/lematin-1922-09-14-a-i0051) | La coopération intellectuelle | 1922-09-14 | lematin; legaulois-1922-09-30-a-i0037 (https://impresso-project.ch/app/article/legaulois-1922-09-30-a-i0037) | Dernière Heure A LA SOCIÉTÉ DES NATIONS | 1922-09-30 | legaulois; legaulois-1922-09-14-a-i0018 (https://impresso-project.ch/app/article/legaulois-1922-09-14-a-i0018) | A LA SOCIÉTÉ DES NATIONS | 1922-09-14 | legaulois; legaulois-1922-09-23-a-i0028 (https://impresso-project.ch/app/article/legaulois-1922-09-23-a-i0028) | EiteSas lirai» | 1922-09-23 | legaulois; EXP-1922-09-14-a-i0100 (https://impresso-project.ch/app/article/EXP-1922-09-14-a-i0100) | DERNIERES DEPECHES | 1922-09-14 | EXP; indeplux-1922-08-29-a-i0081 (https://impresso-project.ch/app/article/indeplux-1922-08-29-a-i0081) | Les Fêtes d’Arlon | 1922-08-29 | indeplux; legaulois-1922-09-29-a-i0025 (https://impresso-project.ch/app/article/legaulois-1922-09-29-a-i0025) | A LA SOCIÉTÉ DES HATIONS | 1922-09-29 | legaulois; GDL-1922-08-28-a-i0055 (https://impresso-project.ch/app/article/GDL-1922-08-28-a-i0055) | LES LIVRES | 1922-08-28 | GDL; legaulois-1922-08-28-a-i0005 (https://impresso-project.ch/app/article/legaulois-1922-08-28-a-i0005) | DANS LES CERCLES | 1922-08-28 | legaulois; oeuvre-1922-08-04-a-i0025 (https://impresso-project.ch/app/article/oeuvre-1922-08-04-a-i0025) | La défense des "humanités" | 1922-08-04 | oeuvre; GDL-1922-08-09-a-i0014 (https://impresso-project.ch/app/article/GDL-1922-08-09-a-i0014) | S. d. | 1922-08-09 | GDL; JDG-1922-08-07-a-i0003 (https://impresso-project.ch/app/article/JDG-1922-08-07-a-i0003) | Influence de l'habitude | 1922-08-07 | JDG; JDG-1922-09-05-a-i0003 (https://impresso-project.ch/app/article/JDG-1922-09-05-a-i0003) | Lettre de Paris | 1922-09-05 | JDG; legaulois-1922-10-06-a-i0056 (https://impresso-project.ch/app/article/legaulois-1922-10-06-a-i0056) | Les Échos | 1922-10-06 | legaulois; GDL-1922-09-16-a-i0067 (https://impresso-project.ch/app/article/GDL-1922-09-16-a-i0067) | Chronique de la S. d. N | 1922-09-16 | GDL; JDG-1922-08-14-a-i0006 (https://impresso-project.ch/app/article/JDG-1922-08-14-a-i0006) | A propos du paradoxe d'Einstein | 1922-08-14 | JDG; JDG-1922-09-15-a-i0024 (https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0024) | Séance plénière | 1922-09-15 | JDG; oeuvre-1922-08-16-a-i0067 (https://impresso-project.ch/app/article/oeuvre-1922-08-16-a-i0067) | La Vie philosophique : Durée et simultanéité. A propos de la théorie d[...] | 1922-08-16 | oeuvre; legaulois-1922-08-06-a-i0008 (https://impresso-project.ch/app/article/legaulois-1922-08-06-a-i0008) | PETIT CARNET | 1922-08-06 | legaulois; JDG-1922-09-16-a-i0020 (https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0020) | Dans les Commissions | 1922-09-16 | JDG; EXP-1922-08-24-a-i0013 (https://impresso-project.ch/app/article/EXP-1922-08-24-a-i0013) | [Sans titre] | 1922-08-24 | EXP; lepetitparisien-1922-08-04-a-i0056 (https://impresso-project.ch/app/article/lepetitparisien-1922-08-04-a-i0056) | LE DONJON DE VINCENNES SEfHUWL TRANSFORME EN BIBLIOTHÈQUE INTERNATIONA[...] | 1922-08-04 | lepetitparisien; legaulois-1922-10-26-a-i0051 (https://impresso-project.ch/app/article/legaulois-1922-10-26-a-i0051) | Les Cinq Académies | 1922-10-26 | legaulois; IMP-1922-08-26-a-i0023 (https://impresso-project.ch/app/article/IMP-1922-08-26-a-i0023) | Chronique suisse | 1922-08-26 | IMP; lepetitparisien-1922-08-01-a-i0029 (https://impresso-project.ch/app/article/lepetitparisien-1922-08-01-a-i0029) | LE COMITÉ DE COOPÉRATION INTELLECTUELLE SE RÉUNIT AUJOURD'HUI A GENÈVE | 1922-08-01 | lepetitparisien; legaulois-1922-10-13-a-i0034 (https://impresso-project.ch/app/article/legaulois-1922-10-13-a-i0034) | Les Échos | 1922-10-13 | legaulois; legaulois-1922-08-04-a-i0023 (https://impresso-project.ch/app/article/legaulois-1922-08-04-a-i0023) | Les Échos | 1922-08-04 | legaulois; legaulois-1922-09-30-a-i0011 (https://impresso-project.ch/app/article/legaulois-1922-09-30-a-i0011) | PETIT CARNET | 1922-09-30 | legaulois; GDL-1922-09-14-a-i0048 (https://impresso-project.ch/app/article/GDL-1922-09-14-a-i0048) | [Sans titre] | 1922-09-14 | GDL; GDL-1922-09-15-a-i0073 (https://impresso-project.ch/app/article/GDL-1922-09-15-a-i0073) | Chronique de la S. d. N. | 1922-09-15 | GDL; EXP-1922-08-08-a-i0046 (https://impresso-project.ch/app/article/EXP-1922-08-08-a-i0046) | Coopération intellectuelle | 1922-08-08 | EXP; GDL-1922-08-02-a-i0002 (https://impresso-project.ch/app/article/GDL-1922-08-02-a-i0002) | Deux commissions de premier plan | 1922-08-02 | GDL; legaulois-1922-08-19-a-i0025 (https://impresso-project.ch/app/article/legaulois-1922-08-19-a-i0025) | LES LIVRES DU JOUR | 1922-08-19 | legaulois; JDG-1922-09-14-a-i0095 (https://impresso-project.ch/app/article/JDG-1922-09-14-a-i0095) | Société des nations XXme session du Conseil | 1922-09-14 | JDG; oeuvre-1922-09-14-a-i0034 (https://impresso-project.ch/app/article/oeuvre-1922-09-14-a-i0034) | UN RAPPORT DE M. BERGSON | 1922-09-14 | oeuvre; EXP-1922-08-10-a-i0021 (https://impresso-project.ch/app/article/EXP-1922-08-10-a-i0021) | [Sans titre] | 1922-08-10 | EXP; legaulois-1922-08-26-a-i0025 (https://impresso-project.ch/app/article/legaulois-1922-08-26-a-i0025) | LES LIVRES DU JOUR | 1922-08-26 | legaulois; oeuvre-1922-10-06-a-i0016 (https://impresso-project.ch/app/article/oeuvre-1922-10-06-a-i0016) | Les mots en suspens | 1922-10-06 | oeuvre; obermosel-1922-08-10-a-i0029 (https://impresso-project.ch/app/article/obermosel-1922-08-10-a-i0029) | Organisierung der internation. geistigen Arbeit. | 1922-08-10 | obermosel; lepetitparisien-1922-09-14-a-i0026 (https://impresso-project.ch/app/article/lepetitparisien-1922-09-14-a-i0026) | LA QUESTION DU PACTE DE GARANTIE | 1922-09-14 | lepetitparisien; oeuvre-1922-09-16-a-i0035 (https://impresso-project.ch/app/article/oeuvre-1922-09-16-a-i0035) | LA COOPÉRATION INTELLECTUELLE | 1922-09-16 | oeuvre; LLE-1922-08-02-a-i0006 (https://impresso-project.ch/app/article/LLE-1922-08-02-a-i0006) | Deux trains allant à Lourdes se tamponne... | 1922-08-02 | LLE; lematin-1922-08-02-a-i0051 (https://impresso-project.ch/app/article/lematin-1922-08-02-a-i0051) | NOUVELLES EN TROIS LIGNES | 1922-08-02 | lematin; GDL-1922-08-06-a-i0074 (https://impresso-project.ch/app/article/GDL-1922-08-06-a-i0074) | Sa £•• | 1922-08-06 | GDL; oeuvre-1922-08-02-a-i0085 (https://impresso-project.ch/app/article/oeuvre-1922-08-02-a-i0085) | La Vie philosophique | 1922-08-02 | oeuvre; GDL-1922-08-26-a-i0026 (https://impresso-project.ch/app/article/GDL-1922-08-26-a-i0026) | CANTON DE VAUD | 1922-08-26 | GDL; NZZ-1922-09-14-b-i0001 (https://impresso-project.ch/app/article/NZZ-1922-09-14-b-i0001) | [Sans titre] | 1922-09-14 | NZZ; LLE-1922-09-16-a-i0090 (https://impresso-project.ch/app/article/LLE-1922-09-16-a-i0090) | SOCIETE DES NATIONS | 1922-09-16 | LLE; LLE-1922-08-26-a-i0101 (https://impresso-project.ch/app/article/LLE-1922-08-26-a-i0101) | Confédération | 1922-08-26 | LLE; NZZ-1922-08-07-b-i0002 (https://impresso-project.ch/app/article/NZZ-1922-08-07-b-i0002) | [Sans titre] | 1922-08-07 | NZZ; NZZ-1922-10-19-b-i0001 (https://impresso-project.ch/app/article/NZZ-1922-10-19-b-i0001) | [Sans titre] | 1922-10-19 | NZZ; LSE-1922-09-22-a-i0001 (https://impresso-project.ch/app/article/LSE-1922-09-22-a-i0001) | Quotidien socialiste | 1922-09-22 | LSE; JDG-1922-08-06-a-i0040 (https://impresso-project.ch/app/article/JDG-1922-08-06-a-i0040) | [Sans titre] | 1922-08-06 | JDG; tageblatt-1922-09-15-a-i0010 (https://impresso-project.ch/app/article/tageblatt-1922-09-15-a-i0010) | Vom Völkerbund.  Nie intellektuelle Arbeit und der Völkerbund. | 1922-09-15 | tageblatt; NZZ-1922-08-01-b-i0002 (https://impresso-project.ch/app/article/NZZ-1922-08-01-b-i0002) | [Sans titre] | 1922-08-01 | NZZ; GDL-1922-08-01-a-i0064 (https://impresso-project.ch/app/article/GDL-1922-08-01-a-i0064) | S.d. N | 1922-08-01 | GDL; NZZ-1922-09-14-b-i0002 (https://impresso-project.ch/app/article/NZZ-1922-09-14-b-i0002) | [Sans titre] | 1922-09-14 | NZZ; NZZ-1922-08-08-a-i0002 (https://impresso-project.ch/app/article/NZZ-1922-08-08-a-i0002) | [Sans titre] | 1922-08-08 | NZZ; LLE-1922-08-09-a-i0007 (https://impresso-project.ch/app/article/LLE-1922-08-09-a-i0007) | Le comité de coopération Intellectuelle | 1922-08-09 | LLE; NZZ-1922-08-05-b-i0002 (https://impresso-project.ch/app/article/NZZ-1922-08-05-b-i0002) | [Sans titre] | 1922-08-05 | NZZ</t>
+  </si>
+  <si>
+    <t>oeuvre-1922-09-23-a-i0036 (https://impresso-project.ch/app/article/oeuvre-1922-09-23-a-i0036) | Le rapatriement des prisonniers de guerre | 1922-09-23 | oeuvre; LLE-1922-08-25-a-i0008 (https://impresso-project.ch/app/article/LLE-1922-08-25-a-i0008) | SOCIÉTÉ DES NATIONS | 1922-08-25 | LLE; JDG-1922-09-16-a-i0010 (https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0010) | Société des nations | 1922-09-16 | JDG; JDG-1922-09-20-a-i0001 (https://impresso-project.ch/app/article/JDG-1922-09-20-a-i0001) | [Sans titre] | 1922-09-20 | JDG; JDG-1922-09-25-a-i0039 (https://impresso-project.ch/app/article/JDG-1922-09-25-a-i0039) | [Sans titre] | 1922-09-25 | JDG; JDG-1922-09-23-a-i0015 (https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0015) | Assemblée de la Société des nations | 1922-09-23 | JDG; lepetitparisien-1922-08-24-a-i0030 (https://impresso-project.ch/app/article/lepetitparisien-1922-08-24-a-i0030) | M. Louis de Brouckère est nommé délégué belge à la S. D. N. | 1922-08-24 | lepetitparisien; JDG-1922-09-26-a-i0084 (https://impresso-project.ch/app/article/JDG-1922-09-26-a-i0084) | g me EDITION Assemblée de la Société des nations | 1922-09-26 | JDG; JDG-1922-09-07-a-i0036 (https://impresso-project.ch/app/article/JDG-1922-09-07-a-i0036) | Dans les commissions | 1922-09-07 | JDG; tageblatt-1922-09-05-a-i0034 (https://impresso-project.ch/app/article/tageblatt-1922-09-05-a-i0034) | PETITS COUPS D'ÊPINGLE. | 1922-09-05 | tageblatt; JDG-1922-09-16-a-i0018 (https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0018) | Un télégramme du Brésil. — Pour la Géorgi e | 1922-09-16 | JDG; indeplux-1922-08-24-a-i0022 (https://impresso-project.ch/app/article/indeplux-1922-08-24-a-i0022) | La S. d. N. | 1922-08-24 | indeplux; JDG-1922-09-27-a-i0042 (https://impresso-project.ch/app/article/JDG-1922-09-27-a-i0042) | L'hommage au soldat belge | 1922-09-27 | JDG; EXP-1922-09-16-a-i0114 (https://impresso-project.ch/app/article/EXP-1922-09-16-a-i0114) | POLITIQUE | 1922-09-16 | EXP; JDG-1922-09-21-a-i0090 (https://impresso-project.ch/app/article/JDG-1922-09-21-a-i0090) | Assemblée de la Société des nations | 1922-09-21 | JDG; lematin-1922-08-08-a-i0046 (https://impresso-project.ch/app/article/lematin-1922-08-08-a-i0046) | Une conférence internationale socialiste à Bruxelles | 1922-08-08 | lematin; JDG-1922-09-03-a-i0043 (https://impresso-project.ch/app/article/JDG-1922-09-03-a-i0043) | Délégués à la troisième assemblée | 1922-09-03 | JDG; lematin-1922-08-24-a-i0056 (https://impresso-project.ch/app/article/lematin-1922-08-24-a-i0056) | NOUVELLES EN TROIS LIGNES | 1922-08-24 | lematin; EXP-1922-09-04-a-i0040 (https://impresso-project.ch/app/article/EXP-1922-09-04-a-i0040) | ; ;•,;. POLITIQUE | 1922-09-04 | EXP; FZG-1922-09-21-a-i0018 (https://impresso-project.ch/app/article/FZG-1922-09-21-a-i0018) | • Neueste Meldunge« » | 1922-09-21 | FZG</t>
+  </si>
+  <si>
+    <t>lematin-1922-08-30-a-i0036 (https://impresso-project.ch/app/article/lematin-1922-08-30-a-i0036) | La Bulgarie envoie une mission secrète à Moscou | 1922-08-30 | lematin; GDL-1922-08-31-a-i0024 (https://impresso-project.ch/app/article/GDL-1922-08-31-a-i0024) | S^a VH &amp; | 1922-08-31 | GDL; lematin-1922-08-31-a-i0068 (https://impresso-project.ch/app/article/lematin-1922-08-31-a-i0068) | M. Todoroff n'ira pas à Moscou | 1922-08-31 | lematin</t>
+  </si>
+  <si>
+    <t>legaulois-1922-09-28-a-i0009 (https://impresso-project.ch/app/article/legaulois-1922-09-28-a-i0009) | DANS LE MONDE OFFICIEL | 1922-09-28 | legaulois</t>
   </si>
   <si>
     <t>Suisse</t>
@@ -869,11 +920,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1177,48 +1228,48 @@
   <cols>
     <col min="1" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1"/>
-    <col min="8" max="8" width="80.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="100.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1232,30 +1283,29 @@
       <c r="C2" t="s">
         <v>83</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H2" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-27-a-i0029","IMP-1922-09-27-a-i0029") | Bibliographie | 1922-09-27 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-05-a-i0030","JDG-1922-09-05-a-i0030") | Assemblées à la Réformation | 1922-09-05 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-06-a-i0010","JDG-1922-09-06-a-i0010") | Lettre de Finlande | 1922-09-06 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-28-a-i0045","JDG-1922-09-28-a-i0045") | [Sans titre] | 1922-09-28 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-18-a-i0044","lepetitparisien-1922-08-18-a-i0044") | LE XIV3 CONGRÈS UNIVERSEL D'ESPERANTO | 1922-08-18 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/LLS-1922-10-21-a-i0025","LLS-1922-10-21-a-i0025") | Vient de paraître | 1922-10-21 | LLS; =HYPERLINK("https://impresso-project.ch/app/article/LLS-1922-10-07-a-i0020","LLS-1922-10-07-a-i0020") | Vient de paraître | 1922-10-07 | LLS; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-30-a-i0047","JDG-1922-09-30-a-i0047") | PARTI DÉMOCRATIQUE | 1922-09-30 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-09-25-a-i0001","LSE-1922-09-25-a-i0001") | Quotidien socialiste Lecteurs, I’ î socialiste est paru Vive la Démocr[...] | 1922-09-25 | LSE; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-07-b-i0006","NZZ-1922-09-07-b-i0006") | [Sans titre] | 1922-09-07 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-09-22-a-i0025","LSE-1922-09-22-a-i0025") | ETRANGER | 1922-09-22 | LSE; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-10-29-a-i0072","GDL-1922-10-29-a-i0072") | LES LIVRES DU JOUR | 1922-10-29 | GDL</f>
-        <v>0</v>
+      <c r="H2" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="I2" t="s">
-        <v>244</v>
+        <v>261</v>
       </c>
       <c r="J2" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K2" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1268,30 +1318,29 @@
       <c r="C3" t="s">
         <v>84</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H3" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-17-a-i0021","JDG-1922-09-17-a-i0021") | [Sans titre] | 1922-09-17 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-17-a-i0010","GDL-1922-09-17-a-i0010") | Sa Sfs Ma | 1922-09-17 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-09-a-i0027","oeuvre-1922-09-09-a-i0027") | UN GRAND DISCOURS DE LORD BALFOUR | 1922-09-09 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-06-a-i0004","JDG-1922-08-06-a-i0004") | Sous les ombrages d'Academus | 1922-08-06 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-09-06-a-i0027","lepetitparisien-1922-09-06-a-i0027") | La troisième séance de l'Assemblée de la S. D. H | 1922-09-06 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-02-a-i0020","JDG-1922-08-02-a-i0020") | Le proche Orient | 1922-08-02 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-13-a-i0092","JDG-1922-09-13-a-i0092") | gme Société des nations | 1922-09-13 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-22-a-i0079","GDL-1922-09-22-a-i0079") | La troisième session delaJU. N. | 1922-09-22 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-06-a-i0025","JDG-1922-09-06-a-i0025") | LA QUATRIEME SEANCE | 1922-09-06 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-29-a-i0004","GDL-1922-09-29-a-i0004") | La troisième session de la S. d. N. Vingtième séance plénière | 1922-09-29 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-22-a-i0029","JDG-1922-09-22-a-i0029") | Contre l'esclavage | 1922-09-22 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-07-a-i0015","JDG-1922-09-07-a-i0015") | Société des nations | 1922-09-07 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-13-a-i0039","indeplux-1922-09-13-a-i0039") | Société des Nations La Société des Nations au travail | 1922-09-13 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-22-a-i0093","oeuvre-1922-09-22-a-i0093") | L'ASSEMBLÉE DE LA SOCIÉTÉ DES NATIONS s'occupe de la protection des mi[...] | 1922-09-22 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-15-a-i0030","oeuvre-1922-09-15-a-i0030") | A GENÈVE, PENDANT L'ENTR'ACTE : Le projet de Lord Robert Cecil a fait [...] | 1922-09-15 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-10-11-a-i0002","LSE-1922-10-11-a-i0002") | EN EUROPE CENTRALE Aux Chambres féd | 1922-10-11 | LSE; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-03-a-i0012","GDL-1922-08-03-a-i0012") | Sa fia. Ni | 1922-08-03 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-23-a-i0002","NZZ-1922-09-23-a-i0002") | [Sans titre] | 1922-09-23 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-09-15-a-i0001","LSE-1922-09-15-a-i0001") | Quotidien socialiste |OT~Citoyens suisses, ne vous laissez pas museler[...] | 1922-09-15 | LSE; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-14-a-i0011","GDL-1922-09-14-a-i0011") | 9B ÊEB NB | 1922-09-14 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-29-c-i0002","NZZ-1922-09-29-c-i0002") | [Sans titre] | 1922-09-29 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-10-10-a-i0001","LSE-1922-10-10-a-i0001") | La Sentinelle Quotidien socialiste Lecteurs, achetez de préférence l’Â[...] | 1922-10-10 | LSE; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-21-a-i0010","NZZ-1922-09-21-a-i0010") | [Sans titre] | 1922-09-21 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-21-a-i0002","NZZ-1922-09-21-a-i0002") | [Sans titre] | 1922-09-21 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-15-b-i0001","NZZ-1922-09-15-b-i0001") | [Sans titre] | 1922-09-15 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-11-b-i0014","NZZ-1922-09-11-b-i0014") | [Sans titre] | 1922-09-11 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-26-c-i0002","NZZ-1922-09-26-c-i0002") | [Sans titre] | 1922-09-26 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-09-07-a-i0006","LLE-1922-09-07-a-i0006") | Société des nations | 1922-09-07 | LLE</f>
-        <v>0</v>
+      <c r="H3" s="1" t="s">
+        <v>245</v>
       </c>
       <c r="I3" t="s">
-        <v>245</v>
+        <v>262</v>
       </c>
       <c r="J3" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K3" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1304,30 +1353,29 @@
       <c r="C4" t="s">
         <v>85</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H4" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-21-a-i0029","JDG-1922-08-21-a-i0029") | CARNET DU JOUR | 1922-08-21 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/LES-1922-08-19-a-i0010","LES-1922-08-19-a-i0010") | Le Bureau International raueaiion | 1922-08-19 | LES; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-06-a-i0011","GDL-1922-08-06-a-i0011") | S&amp;gt; dL ra | 1922-08-06 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-23-a-i0044","JDG-1922-08-23-a-i0044") | [Sans titre] | 1922-08-23 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-20-a-i0054","JDG-1922-08-20-a-i0054") | CARNET DU JOUR | 1922-08-20 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0040","JDG-1922-09-16-a-i0040") | [Sans titre] | 1922-09-16 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-17-a-i0054","JDG-1922-09-17-a-i0054") | ÛEiÈWE | 1922-09-17 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-15-a-i0041","JDG-1922-08-15-a-i0041") | CARNET DU JOUR | 1922-08-15 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-19-a-i0045","JDG-1922-08-19-a-i0045") | GENÈVE | 1922-08-19 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-11-a-i0042","JDG-1922-08-11-a-i0042") | GENÈV E | 1922-08-11 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-05-a-i0017","JDG-1922-08-05-a-i0017") | Société des dations | 1922-08-05 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-11-a-i0043","JDG-1922-08-11-a-i0043") | CARNET DU JOUR | 1922-08-11 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-13-a-i0043","JDG-1922-08-13-a-i0043") | GENÈVE | 1922-08-13 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-19-a-i0048","JDG-1922-08-19-a-i0048") | CARNET DU JOUR | 1922-08-19 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-13-d-i0001","NZZ-1922-08-13-d-i0001") | [Sans titre] | 1922-08-13 | NZZ</f>
-        <v>0</v>
+      <c r="H4" s="1" t="s">
+        <v>246</v>
       </c>
       <c r="I4" t="s">
-        <v>246</v>
+        <v>263</v>
       </c>
       <c r="J4" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K4" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1340,27 +1388,26 @@
       <c r="C5" t="s">
         <v>86</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H5" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-10-16-a-i0001","indeplux-1922-10-16-a-i0001") | Billet extérieur | 1922-10-16 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-04-a-i0001","indeplux-1922-09-04-a-i0001") | Billet extérieur | 1922-09-04 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-18-a-i0001","indeplux-1922-09-18-a-i0001") | Billet extérieur | 1922-09-18 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-10-30-a-i0001","indeplux-1922-10-30-a-i0001") | Billet extérieur | 1922-10-30 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-16-a-i0001","indeplux-1922-08-16-a-i0001") | Billet extérieur | 1922-08-16 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-10-23-a-i0001","indeplux-1922-10-23-a-i0001") | Billet extérieur | 1922-10-23 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-10-09-a-i0001","indeplux-1922-10-09-a-i0001") | Billet extérieur | 1922-10-09 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-21-a-i0001","indeplux-1922-08-21-a-i0001") | Billet extérieur | 1922-08-21 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-13-a-i0001","indeplux-1922-09-13-a-i0001") | Billet extérieur | 1922-09-13 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-28-a-i0001","indeplux-1922-08-28-a-i0001") | Billet extérieur | 1922-08-28 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-25-a-i0001","indeplux-1922-09-25-a-i0001") | Billet extérieur | 1922-09-25 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-08-a-i0001","indeplux-1922-08-08-a-i0001") | Billet extérieur | 1922-08-08 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-02-a-i0094","EXP-1922-09-02-a-i0094") | POLITIQUE , | 1922-09-02 | EXP</f>
-        <v>0</v>
+      <c r="H5" s="1" t="s">
+        <v>247</v>
       </c>
       <c r="I5" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="J5" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K5" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1373,30 +1420,29 @@
       <c r="C6" t="s">
         <v>87</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="H6" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-21-a-i0020","GDL-1922-08-21-a-i0020") | 9B CB Sa | 1922-08-21 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-23-a-i0019","indeplux-1922-08-23-a-i0019") | M. Léon Bérard et l’Espéranto | 1922-08-23 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-24-a-i0070","lepetitparisien-1922-08-24-a-i0070") | L'ESPÉRANTO | 1922-08-24 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-25-a-i0005","NZZ-1922-09-25-a-i0005") | [Sans titre] | 1922-09-25 | NZZ</f>
-        <v>0</v>
+      <c r="H6" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="I6" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="J6" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K6" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1409,27 +1455,26 @@
       <c r="C7" t="s">
         <v>88</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H7" s="2"/>
       <c r="I7" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="J7" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="K7" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1442,24 +1487,23 @@
       <c r="C8" t="s">
         <v>89</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H8" s="2"/>
       <c r="I8" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="J8" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="K8" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1472,27 +1516,26 @@
       <c r="C9" t="s">
         <v>90</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H9" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-24-a-i0049","EXP-1922-08-24-a-i0049") | POLITIQUE | 1922-08-24 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-23-a-i0107","JDG-1922-08-23-a-i0107") | Société des Nations | 1922-08-23 | JDG</f>
-        <v>0</v>
+      <c r="H9" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="I9" t="s">
         <v>58</v>
       </c>
       <c r="J9" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="K9" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1505,30 +1548,29 @@
       <c r="C10" t="s">
         <v>91</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="H10" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-13-a-i0069","EXP-1922-09-13-a-i0069") | POLITIQUE Société des nations | 1922-09-13 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-13-a-i0020","JDG-1922-09-13-a-i0020") | Société des nations | 1922-09-13 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-09-20-a-i0031","oecaen-1922-09-20-a-i0031") | &lt; LA FXiBCHB | 1922-09-20 | oecaen; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-19-a-i0026","oeuvre-1922-09-19-a-i0026") | LA DIXIÈME ASSAMBLEE PLÊNIÈRE | 1922-09-19 | oeuvre</f>
-        <v>0</v>
+      <c r="H10" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="I10" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="J10" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="K10" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1541,27 +1583,26 @@
       <c r="C11" t="s">
         <v>92</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="H11" s="2"/>
       <c r="I11" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="J11" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K11" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1574,27 +1615,26 @@
       <c r="C12" t="s">
         <v>93</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H12" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-08-05-a-i0034","oeuvre-1922-08-05-a-i0034") | L'Amérique et la Société des Nations | 1922-08-05 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-17-a-i0074","GDL-1922-08-17-a-i0074") | [Sans titre] | 1922-08-17 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-17-a-i0083","JDG-1922-08-17-a-i0083") | Société des Nations | 1922-08-17 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-19-a-i0039","lematin-1922-09-19-a-i0039") | Les secours aux réfugiés de Smyrne | 1922-09-19 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-10-a-i0016","JDG-1922-09-10-a-i0016") | DISCUSSIO N GENERAL E SU R L E RAPPOR T D U CONSEI L | 1922-09-10 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-10-27-a-i0044","JDG-1922-10-27-a-i0044") | IV me C©nféreisce du îravai | 1922-10-27 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-19-a-i0090","JDG-1922-09-19-a-i0090") | S me EDITION Société des nations | 1922-09-19 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-18-a-i0035","EXP-1922-08-18-a-i0035") | POLITIQUE | 1922-08-18 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-10-02-a-i0020","JDG-1922-10-02-a-i0020") | Société des nations | 1922-10-02 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-04-a-i0071","GDL-1922-09-04-a-i0071") | Sa da | 1922-09-04 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-10-03-a-i0004","legaulois-1922-10-03-a-i0004") | DANS LE MONDE OFFICIEL | 1922-10-03 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-04-a-i0056","EXP-1922-09-04-a-i0056") | APOLITIQUE | 1922-09-04 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-29-a-i0010","GDL-1922-09-29-a-i0010") | L'Azerbaïdjan et la S. d. | 1922-09-29 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-19-a-i0002","NZZ-1922-09-19-a-i0002") | [Sans titre] | 1922-09-19 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-09-05-a-i0002","LLE-1922-09-05-a-i0002") | La troisième assemblée de la Société des... | 1922-09-05 | LLE; =HYPERLINK("https://impresso-project.ch/app/article/luxwort-1922-09-05-a-i0058","luxwort-1922-09-05-a-i0058") | Die 3. Völkerbundsversammlung in Genf. | 1922-09-05 | luxwort; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-03-a-i0002","NZZ-1922-09-03-a-i0002") | [Sans titre] | 1922-09-03 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-08-18-a-i0038","FZG-1922-08-18-a-i0038") | «danken die schwerste «Niederlage. «Gin ... | 1922-08-18 | FZG; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-10-23-d-i0001","NZZ-1922-10-23-d-i0001") | [Sans titre] | 1922-10-23 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-10-24-a-i0014","FZG-1922-10-24-a-i0014") | mmmm W&gt;/AL- rMsh*.*.*» A. •*&amp; Jts-**i | 1922-10-24 | FZG; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-03-a-i0009","NZZ-1922-09-03-a-i0009") | [Sans titre] | 1922-09-03 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-09-04-a-i0015","FZG-1922-09-04-a-i0015") | • Neueste Meldunam # | 1922-09-04 | FZG; =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-09-02-a-i0022","FZG-1922-09-02-a-i0022") | Jum griechisch«türkische Konflikt. Adana... | 1922-09-02 | FZG</f>
-        <v>0</v>
+      <c r="H12" s="1" t="s">
+        <v>251</v>
       </c>
       <c r="I12" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="J12" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K12" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1607,30 +1647,29 @@
       <c r="C13" t="s">
         <v>94</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H13" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-22-a-i0018","indeplux-1922-09-22-a-i0018") | Société des Nations Une note exprimant les vœux de la France sera prés[...] | 1922-09-22 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-12-a-i0025","legaulois-1922-09-12-a-i0025") | Réponse de lord Robert Cecil | 1922-09-12 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-14-a-i0036","oeuvre-1922-09-14-a-i0036") | M. LLOYD GEORGE VIENDRA-T-IL A GENÈVE ? | 1922-09-14 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-08-a-i0066","EXP-1922-09-08-a-i0066") | POLITIQUE Société des Nations | 1922-09-08 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-10-08-a-i0033","oeuvre-1922-10-08-a-i0033") | Le Dr Nansen organise une mission purement britannique | 1922-10-08 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-20-a-i0027","oeuvre-1922-09-20-a-i0027") | LE PROBLÈME DES RÉPARATIONS | 1922-09-20 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-23-a-i0032","legaulois-1922-09-23-a-i0032") | A LA SOCIÉTÉ DES MATIONS | 1922-09-23 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-01-a-i0016","legaulois-1922-09-01-a-i0016") | Dernière Heure Â la Société des Nations | 1922-09-01 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-14-a-i0046","indeplux-1922-09-14-a-i0046") | Un accord intervient entre lord Robert ( ecil et M. de Jouvenel au suj[...] | 1922-09-14 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-23-a-i0030","indeplux-1922-09-23-a-i0030") | Le point de vue français sur le désarmement | 1922-09-23 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-13-a-i0057","lematin-1922-09-13-a-i0057") | La commission adopté le projet de lord Robert Cecil sur le désarmement | 1922-09-13 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0010","JDG-1922-09-09-a-i0010") | LÀ SITUATION | 1922-09-09 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-08-a-i0001","JDG-1922-09-08-a-i0001") | BULLETIN | 1922-09-08 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-19-a-i0014","legaulois-1922-09-19-a-i0014") | A la Société des Nations | 1922-09-19 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-14-a-i0023","legaulois-1922-09-14-a-i0023") | Vers un pacte de garantie | 1922-09-14 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-07-a-i0045","legaulois-1922-09-07-a-i0045") | Le Chancelier d'Autriche expose la détresse de son pays | 1922-09-07 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-23-a-i0037","lematin-1922-09-23-a-i0037") | LaS.D.N. s'occupe du conflit gréco-turc | 1922-09-23 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-09-12-a-i0032","lepetitparisien-1922-09-12-a-i0032") | A L'ASSEMBLÉE de la Société des Nations | 1922-09-12 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0017","JDG-1922-09-09-a-i0017") | M. Sciai oj? | 1922-09-09 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-23-a-i0039","oeuvre-1922-09-23-a-i0039") | La question d'Orient | 1922-09-23 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-16-a-i0031","lematin-1922-09-16-a-i0031") | La réduction des armements doit dépendre des garanties données par le [...] | 1922-09-16 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-18-a-i0049","EXP-1922-09-18-a-i0049") | 1POLITIQUE&amp;gt;£.i | 1922-09-18 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-12-a-i0002","IMP-1922-09-12-a-i0002") | ba Semaine internationale | 1922-09-12 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0008","JDG-1922-09-09-a-i0008") | t&amp;UrcS | 1922-09-09 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-10-03-a-i0092","EXP-1922-10-03-a-i0092") | Chronique parlementaire | 1922-10-03 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-23-a-i0051","indeplux-1922-09-23-a-i0051") | DERNIÈRE HEURE | 1922-09-23 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-10-03-a-i0001","IMP-1922-10-03-a-i0001") | L&amp;gt;a Semaine internationale | 1922-10-03 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-17-a-i0038","lematin-1922-09-17-a-i0038") | Un émouvant débat entre le délégué français et le délégué anglais | 1922-09-17 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-10-12-a-i0008","oeuvre-1922-10-12-a-i0008") | M. Lloyd George prépare contre ses détracteurs une grande bataille | 1922-10-12 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-01-a-i0001","JDG-1922-09-01-a-i0001") | [Sans titre] | 1922-09-01 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-28-a-i0001","JDG-1922-09-28-a-i0001") | [Sans titre] | 1922-09-28 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-23-a-i0043","EXP-1922-08-23-a-i0043") | POLITIQUE | 1922-08-23 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-17-a-i0019","legaulois-1922-09-17-a-i0019") | Dernière A LA SOCIÉTÉ DES NATIONS | 1922-09-17 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-18-a-i0018","legaulois-1922-09-18-a-i0018") | Dernière Heure AU SOCIÉTÉ DES MATIONS | 1922-09-18 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-21-a-i0061","GDL-1922-09-21-a-i0061") | La troisième session de la S. d. N. | 1922-09-21 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-14-a-i0059","GDL-1922-09-14-a-i0059") | Chronique de la S. d.N | 1922-09-14 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-10-06-a-i0093","EXP-1922-10-06-a-i0093") | Après la session | 1922-10-06 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-08-a-i0034","legaulois-1922-09-08-a-i0034") | A LA SOCIÉTÉ DES KATIONS | 1922-09-08 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-12-a-i0024","legaulois-1922-09-12-a-i0024") | A LA SOCIÉTÉ DES NATIONS | 1922-09-12 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-13-a-i0077","lematin-1922-09-13-a-i0077") | LA PROCHAINE ARRIVÉE DE M. LLOYD GEORGE A GENÈVE | 1922-09-13 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0090","JDG-1922-09-15-a-i0090") | Le plan Cecil et la doctrine d e Monroë | 1922-09-15 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-13-a-i0043","EXP-1922-09-13-a-i0043") | POLITIQUE Société des ffati _ * __§ | 1922-09-13 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-23-a-i0012","GDL-1922-08-23-a-i0012") | S. | 1922-08-23 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0006","JDG-1922-09-15-a-i0006") | BULLETIN | 1922-09-15 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-10-05-a-i0006","JDG-1922-10-05-a-i0006") | Chronique parlementaire | 1922-10-05 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-22-a-i0010","JDG-1922-09-22-a-i0010") | [Sans titre] | 1922-09-22 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-13-a-i0074","EXP-1922-09-13-a-i0074") | DERNIERES REPÊCHES | 1922-09-13 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-15-a-i0053","lematin-1922-09-15-a-i0053") | Le délégué français propose, comme première mesure de réduire les dépe[...] | 1922-09-15 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-22-a-i0051","EXP-1922-09-22-a-i0051") | Sodttè des nations | 1922-09-22 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-28-a-i0029","IMP-1922-09-28-a-i0029") | Ledésarmement devant l'Assemblée de Genève | 1922-09-28 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-28-a-i0054","legaulois-1922-09-28-a-i0054") | h la Société des gâtions | 1922-09-28 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-20-a-i0026","oeuvre-1922-09-20-a-i0026") | LE PACTE DE GARANTIE | 1922-09-20 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-14-a-i0020","JDG-1922-09-14-a-i0020") | L'attitude de l'Argentine | 1922-09-14 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-20-a-i0090","JDG-1922-09-20-a-i0090") | Société des nations | 1922-09-20 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0002","JDG-1922-09-23-a-i0002") | GENEVE, 22 septembre 1922 TJX.LETIN | 1922-09-23 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0073","JDG-1922-09-16-a-i0073") | 2me EDITION....III Société des nations | 1922-09-16 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-20-a-i0025","legaulois-1922-09-20-a-i0025") | A LA SOCIÉTÉ DES NATIONS | 1922-09-20 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-09-a-i0004","GDL-1922-09-09-a-i0004") | La troisième session de la S. d. N. | 1922-09-09 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-14-a-i0050","lematin-1922-09-14-a-i0050") | Le pacte de garantie n'affectera aucunement les traités de paix | 1922-09-14 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-17-a-i0113","JDG-1922-09-17-a-i0113") | gme EDITION ^•.IH.,.1.1.1— i •• - ...M..,,.,— •• '- • IM.-H..MI.III So[...] | 1922-09-17 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-09-03-a-i0039","lepetitparisien-1922-09-03-a-i0039") | La troisième assemblée de la Société des nations | 1922-09-03 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-14-a-i0043","indeplux-1922-09-14-a-i0043") | La Commission du Désarmement discute la proposition de pacte de garant[...] | 1922-09-14 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-28-a-i0039","indeplux-1922-09-28-a-i0039") | Société des Nations La discussion sur la réduction des armements se po[...] | 1922-09-28 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-27-a-i0030","lematin-1922-09-27-a-i0030") | Quand donc l'humanité "* , » nous apportant le pacte de garantie, dira[...] | 1922-09-27 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-09-19-a-i0034","oecaen-1922-09-19-a-i0034") | UN NOUVEAU TEXTE | 1922-09-19 | oecaen; =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-09-27-a-i0006","oecaen-1922-09-27-a-i0006") | Les travaux de la Commission du Désarmement devant l'Assemblée | 1922-09-27 | oecaen; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-13-a-i0002","JDG-1922-09-13-a-i0002") | fc&amp;S | 1922-09-13 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-27-a-i0004","GDL-1922-09-27-a-i0004") | La troisième session aelaJjLd.ll. Dix-septième séance plénière | 1922-09-27 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-26-a-i0038","legaulois-1922-08-26-a-i0038") | Revue de la Presse | 1922-08-26 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-06-a-i0059","EXP-1922-09-06-a-i0059") | POLITIQUE Société cS@s Nattons | 1922-09-06 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-09-09-a-i0056","lepetitparisien-1922-09-09-a-i0056") | CE QUE LA FRANCE A FAIT pour diminuer ses armements | 1922-09-09 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-31-a-i0027","indeplux-1922-08-31-a-i0027") | Une proposition de lord Robert Cecil au sujet du désarmement | 1922-08-31 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-10-25-a-i0001","oeuvre-1922-10-25-a-i0001") | POUR QUE L'ENTENTE REDEVIENNE CORDIALE : Définissons nos « buts de pai[...] | 1922-10-25 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-23-a-i0038","oeuvre-1922-09-23-a-i0038") | Un foyer national pour les Arméniens | 1922-09-23 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0015","JDG-1922-09-09-a-i0015") | Assemblée de fa Société des nations | 1922-09-09 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0099","JDG-1922-09-23-a-i0099") | TROISIEME EDITION La guerre en Asie Mineure et le problème du proche O[...] | 1922-09-23 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-21-a-i0027","JDG-1922-09-21-a-i0027") | Dans les Commissions | 1922-09-21 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-13-a-i0021","legaulois-1922-09-13-a-i0021") | A LA SOCIÉTÉ DES NATIONS | 1922-09-13 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-27-a-i0005","JDG-1922-09-27-a-i0005") | Assemblée de la Société des nations Séance plénière d | 1922-09-27 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-10-28-a-i0069","EXP-1922-10-28-a-i0069") | COÏÏREÎER FRANÇAIS | 1922-10-28 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-04-a-i0003","IMP-1922-09-04-a-i0003") | Lettre de Genève | 1922-09-04 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-18-a-i0089","lematin-1922-09-18-a-i0089") | L'opinion de lord Robert Ceci! sur l'admission du Reich dans la S. D. [...] | 1922-09-18 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-09-18-a-i0016","oecaen-1922-09-18-a-i0016") | Lord Robert Cecfl est partisan de l'admission de l'Allemagne à la SM. | 1922-09-18 | oecaen; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-06-a-i0012","indeplux-1922-09-06-a-i0012") | L’Assemblée de la S. d. N. | 1922-09-06 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-01-a-i0002","lematin-1922-09-01-a-i0002") | M. Lloyd George ira-t-il à Genève? | 1922-09-01 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-21-a-i0038","oeuvre-1922-09-21-a-i0038") | Comment la Belgique négociera les bons allemands | 1922-09-21 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-10-01-a-i0025","lepetitparisien-1922-10-01-a-i0025") | LA SOCIÉTÉ DES NATIONS a clos hier ses travaux | 1922-10-01 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-04-a-i0008","indeplux-1922-09-04-a-i0008") | La Commission approuve le projet de lord Robert Cecil sur le desarmeme[...] | 1922-09-04 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-16-a-i0021","legaulois-1922-09-16-a-i0021") | SHAKESPEARE Fils de la Reine Elisabeth | 1922-09-16 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0004","JDG-1922-09-23-a-i0004") | L'Allemagne et ia Société des nations | 1922-09-23 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-26-a-i0002","IMP-1922-09-26-a-i0002") | ba Semaine internationale | 1922-09-26 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-04-a-i0062","legaulois-1922-08-04-a-i0062") | Le débat à la Chambre des Communes | 1922-08-04 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-08-a-i0006","GDL-1922-09-08-a-i0006") | La troisième session de la S. d. N. | 1922-09-08 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-14-a-i0094","EXP-1922-09-14-a-i0094") | \. POLITIQUE Société des nations | 1922-09-14 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-09-07-a-i0028","indeplux-1922-09-07-a-i0028") | Un discours de lord Robert Cecil | 1922-09-07 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-15-a-i0026","legaulois-1922-09-15-a-i0026") | Les Journaux du matin | 1922-09-15 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-21-a-i0035","legaulois-1922-09-21-a-i0035") | Les Journaux du matin | 1922-09-21 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-18-a-i0060","GDL-1922-09-18-a-i0060") | 9a fia Ni | 1922-09-18 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-20-a-i0041","lematin-1922-09-20-a-i0041") | M. de Jouvenel fait, an nom de la délégation française ' I' .. v" une [...] | 1922-09-20 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-10-20-a-i0051","lematin-1922-10-20-a-i0051") | LES GRANDS RETOURS | 1922-10-20 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-09-a-i0026","IMP-1922-09-09-a-i0026") | Lettre de Genève | 1922-09-09 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-09-20-a-i0001","IMP-1922-09-20-a-i0001") | ba Semaine internationale | 1922-09-20 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-09-a-i0027","JDG-1922-09-09-a-i0027") | En marge de l'Assemblée Réceptio n officiell e | 1922-09-09 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0083","JDG-1922-09-15-a-i0083") | La guerre en Anatolie et le problème du proche Orient | 1922-09-15 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-06-a-i0071","lematin-1922-09-06-a-i0071") | L'assemblée de Genève nomme ses commissions | 1922-09-06 | lematin</f>
-        <v>0</v>
+      <c r="H13" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="I13" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="J13" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K13" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1643,30 +1682,29 @@
       <c r="C14" t="s">
         <v>95</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="H14" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-10-28-a-i0013","legaulois-1922-10-28-a-i0013") | NÉCROLOGIE | 1922-10-28 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-09-26-a-i0049","oecaen-1922-09-26-a-i0049") | TRIBUNAL CORRECTIONNEL | 1922-09-26 | oecaen; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-22-a-i0053","lepetitparisien-1922-08-22-a-i0053") | LECONORÈS UNIVERSEL D'ESPERANTO | 1922-08-22 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-08-a-i0074","lematin-1922-08-08-a-i0074") | NOUVELLES EN TROIS LIGNES | 1922-08-08 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/oecaen-1922-08-06-a-i0080","oecaen-1922-08-06-a-i0080") | I !MJbv3 | 1922-08-06 | oecaen</f>
-        <v>0</v>
+      <c r="H14" s="1" t="s">
+        <v>253</v>
       </c>
       <c r="I14" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="J14" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K14" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1679,27 +1717,26 @@
       <c r="C15" t="s">
         <v>96</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H15" s="2"/>
       <c r="I15" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="J15" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K15" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1712,27 +1749,26 @@
       <c r="C16" t="s">
         <v>97</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H16" s="2"/>
       <c r="I16" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="J16" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K16" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1745,30 +1781,29 @@
       <c r="C17" t="s">
         <v>98</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H17" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-03-a-i0038","indeplux-1922-08-03-a-i0038") | ITALIE La constitution définitive du ministère Facta | 1922-08-03 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-02-a-i0013","GDL-1922-08-02-a-i0013") | Les consultations de M. Facta | 1922-08-02 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/luxwort-1922-08-03-a-i0001","luxwort-1922-08-03-a-i0001") | Zur Kabinettsumbildung in Italien. | 1922-08-03 | luxwort; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-01-b-i0006","NZZ-1922-08-01-b-i0006") | [Sans titre] | 1922-08-01 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-10-18-a-i0002","NZZ-1922-10-18-a-i0002") | [Sans titre] | 1922-10-18 | NZZ</f>
-        <v>0</v>
+      <c r="H17" s="1" t="s">
+        <v>254</v>
       </c>
       <c r="I17" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="J17" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K17" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1781,27 +1816,26 @@
       <c r="C18" t="s">
         <v>99</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H18" s="2"/>
       <c r="I18" t="s">
         <v>58</v>
       </c>
       <c r="J18" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K18" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1814,27 +1848,26 @@
       <c r="C19" t="s">
         <v>100</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="H19" s="2"/>
       <c r="I19" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="J19" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K19" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1847,24 +1880,23 @@
       <c r="C20" t="s">
         <v>101</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="H20" s="2"/>
       <c r="I20" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="J20" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K20" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1877,27 +1909,26 @@
       <c r="C21" t="s">
         <v>102</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H21" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-10-09-a-i0021","JDG-1922-10-09-a-i0021") | Société des Nations | 1922-10-09 | JDG</f>
-        <v>0</v>
+      <c r="H21" s="1" t="s">
+        <v>255</v>
       </c>
       <c r="I21" t="s">
-        <v>255</v>
+        <v>272</v>
       </c>
       <c r="J21" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K21" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1910,24 +1941,23 @@
       <c r="C22" t="s">
         <v>103</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="H22" s="2"/>
       <c r="I22" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="J22" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K22" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1940,24 +1970,23 @@
       <c r="C23" t="s">
         <v>104</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="H23" s="2"/>
       <c r="I23" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="J23" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K23" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1970,24 +1999,23 @@
       <c r="C24" t="s">
         <v>105</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="H24" s="2"/>
       <c r="I24" t="s">
         <v>58</v>
       </c>
       <c r="J24" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="K24" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2000,27 +2028,26 @@
       <c r="C25" t="s">
         <v>106</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="H25" s="2"/>
       <c r="I25" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="J25" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K25" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2033,21 +2060,20 @@
       <c r="C26" t="s">
         <v>107</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="H26" s="2"/>
       <c r="I26" t="s">
         <v>58</v>
       </c>
       <c r="J26" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="K26" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -2060,27 +2086,26 @@
       <c r="C27" t="s">
         <v>108</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H27" s="2"/>
       <c r="I27" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="J27" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K27" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2093,27 +2118,26 @@
       <c r="C28" t="s">
         <v>109</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="H28" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/LES-1922-08-05-a-i0020","LES-1922-08-05-a-i0020") | Encore si cette revue dépassait par la r... | 1922-08-05 | LES; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0036","JDG-1922-09-16-a-i0036") | A propos du droit d'auteur | 1922-09-16 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/LCE-1922-09-11-a-i0010","LCE-1922-09-11-a-i0010") | En Suisse Cordages en loysoeoresTravai. Soi C. Kissimg. cordier, Ullle[...] | 1922-09-11 | LCE; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-08-a-i0018","GDL-1922-09-08-a-i0018") | CONFÉDÉRATION | 1922-09-08 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-11-b-i0021","NZZ-1922-09-11-b-i0021") | [Sans titre] | 1922-09-11 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-10-05-a-i0001","NZZ-1922-10-05-a-i0001") | [Sans titre] | 1922-10-05 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-09-04-a-i0019","LLE-1922-09-04-a-i0019") | Les réformes constitutionnelles au Tessi... | 1922-09-04 | LLE; =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-08-26-a-i0017","FZG-1922-08-26-a-i0017") | Schweiz | 1922-08-26 | FZG</f>
-        <v>0</v>
+      <c r="H28" s="1" t="s">
+        <v>256</v>
       </c>
       <c r="I28" t="s">
-        <v>244</v>
+        <v>261</v>
       </c>
       <c r="J28" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K28" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2126,30 +2150,29 @@
       <c r="C29" t="s">
         <v>110</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="H29" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-26-a-i0095","JDG-1922-08-26-a-i0095") | Nos hôtes | 1922-08-26 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-06-a-i0076","lematin-1922-08-06-a-i0076") | Le président de la Confédération helvétique h la Société des nations | 1922-08-06 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-09-14-a-i0051","lematin-1922-09-14-a-i0051") | La coopération intellectuelle | 1922-09-14 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-30-a-i0037","legaulois-1922-09-30-a-i0037") | Dernière Heure A LA SOCIÉTÉ DES NATIONS | 1922-09-30 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-14-a-i0018","legaulois-1922-09-14-a-i0018") | A LA SOCIÉTÉ DES NATIONS | 1922-09-14 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-23-a-i0028","legaulois-1922-09-23-a-i0028") | EiteSas lirai» | 1922-09-23 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-14-a-i0100","EXP-1922-09-14-a-i0100") | DERNIERES DEPECHES | 1922-09-14 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-29-a-i0081","indeplux-1922-08-29-a-i0081") | Les Fêtes d’Arlon | 1922-08-29 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-29-a-i0025","legaulois-1922-09-29-a-i0025") | A LA SOCIÉTÉ DES HATIONS | 1922-09-29 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-28-a-i0055","GDL-1922-08-28-a-i0055") | LES LIVRES | 1922-08-28 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-28-a-i0005","legaulois-1922-08-28-a-i0005") | DANS LES CERCLES | 1922-08-28 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-08-04-a-i0025","oeuvre-1922-08-04-a-i0025") | La défense des "humanités" | 1922-08-04 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-09-a-i0014","GDL-1922-08-09-a-i0014") | S. d. | 1922-08-09 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-07-a-i0003","JDG-1922-08-07-a-i0003") | Influence de l'habitude | 1922-08-07 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-05-a-i0003","JDG-1922-09-05-a-i0003") | Lettre de Paris | 1922-09-05 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-10-06-a-i0056","legaulois-1922-10-06-a-i0056") | Les Échos | 1922-10-06 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-16-a-i0067","GDL-1922-09-16-a-i0067") | Chronique de la S. d. N | 1922-09-16 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-14-a-i0006","JDG-1922-08-14-a-i0006") | A propos du paradoxe d'Einstein | 1922-08-14 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-15-a-i0024","JDG-1922-09-15-a-i0024") | Séance plénière | 1922-09-15 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-08-16-a-i0067","oeuvre-1922-08-16-a-i0067") | La Vie philosophique : Durée et simultanéité. A propos de la théorie d[...] | 1922-08-16 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-06-a-i0008","legaulois-1922-08-06-a-i0008") | PETIT CARNET | 1922-08-06 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0020","JDG-1922-09-16-a-i0020") | Dans les Commissions | 1922-09-16 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-24-a-i0013","EXP-1922-08-24-a-i0013") | [Sans titre] | 1922-08-24 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-04-a-i0056","lepetitparisien-1922-08-04-a-i0056") | LE DONJON DE VINCENNES SEfHUWL TRANSFORME EN BIBLIOTHÈQUE INTERNATIONA[...] | 1922-08-04 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-10-26-a-i0051","legaulois-1922-10-26-a-i0051") | Les Cinq Académies | 1922-10-26 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/IMP-1922-08-26-a-i0023","IMP-1922-08-26-a-i0023") | Chronique suisse | 1922-08-26 | IMP; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-01-a-i0029","lepetitparisien-1922-08-01-a-i0029") | LE COMITÉ DE COOPÉRATION INTELLECTUELLE SE RÉUNIT AUJOURD'HUI A GENÈVE | 1922-08-01 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-10-13-a-i0034","legaulois-1922-10-13-a-i0034") | Les Échos | 1922-10-13 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-04-a-i0023","legaulois-1922-08-04-a-i0023") | Les Échos | 1922-08-04 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-30-a-i0011","legaulois-1922-09-30-a-i0011") | PETIT CARNET | 1922-09-30 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-14-a-i0048","GDL-1922-09-14-a-i0048") | [Sans titre] | 1922-09-14 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-09-15-a-i0073","GDL-1922-09-15-a-i0073") | Chronique de la S. d. N. | 1922-09-15 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-08-a-i0046","EXP-1922-08-08-a-i0046") | Coopération intellectuelle | 1922-08-08 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-02-a-i0002","GDL-1922-08-02-a-i0002") | Deux commissions de premier plan | 1922-08-02 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-19-a-i0025","legaulois-1922-08-19-a-i0025") | LES LIVRES DU JOUR | 1922-08-19 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-14-a-i0095","JDG-1922-09-14-a-i0095") | Société des nations XXme session du Conseil | 1922-09-14 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-14-a-i0034","oeuvre-1922-09-14-a-i0034") | UN RAPPORT DE M. BERGSON | 1922-09-14 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-08-10-a-i0021","EXP-1922-08-10-a-i0021") | [Sans titre] | 1922-08-10 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-08-26-a-i0025","legaulois-1922-08-26-a-i0025") | LES LIVRES DU JOUR | 1922-08-26 | legaulois; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-10-06-a-i0016","oeuvre-1922-10-06-a-i0016") | Les mots en suspens | 1922-10-06 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/obermosel-1922-08-10-a-i0029","obermosel-1922-08-10-a-i0029") | Organisierung der internation. geistigen Arbeit. | 1922-08-10 | obermosel; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-09-14-a-i0026","lepetitparisien-1922-09-14-a-i0026") | LA QUESTION DU PACTE DE GARANTIE | 1922-09-14 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-16-a-i0035","oeuvre-1922-09-16-a-i0035") | LA COOPÉRATION INTELLECTUELLE | 1922-09-16 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-08-02-a-i0006","LLE-1922-08-02-a-i0006") | Deux trains allant à Lourdes se tamponne... | 1922-08-02 | LLE; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-02-a-i0051","lematin-1922-08-02-a-i0051") | NOUVELLES EN TROIS LIGNES | 1922-08-02 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-06-a-i0074","GDL-1922-08-06-a-i0074") | Sa £•• | 1922-08-06 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-08-02-a-i0085","oeuvre-1922-08-02-a-i0085") | La Vie philosophique | 1922-08-02 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-26-a-i0026","GDL-1922-08-26-a-i0026") | CANTON DE VAUD | 1922-08-26 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-14-b-i0001","NZZ-1922-09-14-b-i0001") | [Sans titre] | 1922-09-14 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-09-16-a-i0090","LLE-1922-09-16-a-i0090") | SOCIETE DES NATIONS | 1922-09-16 | LLE; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-08-26-a-i0101","LLE-1922-08-26-a-i0101") | Confédération | 1922-08-26 | LLE; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-07-b-i0002","NZZ-1922-08-07-b-i0002") | [Sans titre] | 1922-08-07 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-10-19-b-i0001","NZZ-1922-10-19-b-i0001") | [Sans titre] | 1922-10-19 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LSE-1922-09-22-a-i0001","LSE-1922-09-22-a-i0001") | Quotidien socialiste | 1922-09-22 | LSE; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-08-06-a-i0040","JDG-1922-08-06-a-i0040") | [Sans titre] | 1922-08-06 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/tageblatt-1922-09-15-a-i0010","tageblatt-1922-09-15-a-i0010") | Vom Völkerbund.  Nie intellektuelle Arbeit und der Völkerbund. | 1922-09-15 | tageblatt; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-01-b-i0002","NZZ-1922-08-01-b-i0002") | [Sans titre] | 1922-08-01 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-01-a-i0064","GDL-1922-08-01-a-i0064") | S.d. N | 1922-08-01 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-09-14-b-i0002","NZZ-1922-09-14-b-i0002") | [Sans titre] | 1922-09-14 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-08-a-i0002","NZZ-1922-08-08-a-i0002") | [Sans titre] | 1922-08-08 | NZZ; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-08-09-a-i0007","LLE-1922-08-09-a-i0007") | Le comité de coopération Intellectuelle | 1922-08-09 | LLE; =HYPERLINK("https://impresso-project.ch/app/article/NZZ-1922-08-05-b-i0002","NZZ-1922-08-05-b-i0002") | [Sans titre] | 1922-08-05 | NZZ</f>
-        <v>0</v>
+      <c r="H29" s="1" t="s">
+        <v>257</v>
       </c>
       <c r="I29" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="J29" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K29" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -2162,24 +2185,23 @@
       <c r="C30" t="s">
         <v>111</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="H30" s="2"/>
       <c r="I30" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="J30" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K30" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2192,27 +2214,26 @@
       <c r="C31" t="s">
         <v>112</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="H31" s="2"/>
       <c r="I31" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="J31" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K31" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -2225,24 +2246,23 @@
       <c r="C32" t="s">
         <v>113</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="H32" s="2"/>
       <c r="I32" t="s">
         <v>58</v>
       </c>
       <c r="J32" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="K32" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -2255,27 +2275,26 @@
       <c r="C33" t="s">
         <v>114</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H33" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/oeuvre-1922-09-23-a-i0036","oeuvre-1922-09-23-a-i0036") | Le rapatriement des prisonniers de guerre | 1922-09-23 | oeuvre; =HYPERLINK("https://impresso-project.ch/app/article/LLE-1922-08-25-a-i0008","LLE-1922-08-25-a-i0008") | SOCIÉTÉ DES NATIONS | 1922-08-25 | LLE; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0010","JDG-1922-09-16-a-i0010") | Société des nations | 1922-09-16 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-20-a-i0001","JDG-1922-09-20-a-i0001") | [Sans titre] | 1922-09-20 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-25-a-i0039","JDG-1922-09-25-a-i0039") | [Sans titre] | 1922-09-25 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-23-a-i0015","JDG-1922-09-23-a-i0015") | Assemblée de la Société des nations | 1922-09-23 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lepetitparisien-1922-08-24-a-i0030","lepetitparisien-1922-08-24-a-i0030") | M. Louis de Brouckère est nommé délégué belge à la S. D. N. | 1922-08-24 | lepetitparisien; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-26-a-i0084","JDG-1922-09-26-a-i0084") | g me EDITION Assemblée de la Société des nations | 1922-09-26 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-07-a-i0036","JDG-1922-09-07-a-i0036") | Dans les commissions | 1922-09-07 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/tageblatt-1922-09-05-a-i0034","tageblatt-1922-09-05-a-i0034") | PETITS COUPS D'ÊPINGLE. | 1922-09-05 | tageblatt; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-16-a-i0018","JDG-1922-09-16-a-i0018") | Un télégramme du Brésil. — Pour la Géorgi e | 1922-09-16 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/indeplux-1922-08-24-a-i0022","indeplux-1922-08-24-a-i0022") | La S. d. N. | 1922-08-24 | indeplux; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-27-a-i0042","JDG-1922-09-27-a-i0042") | L'hommage au soldat belge | 1922-09-27 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-16-a-i0114","EXP-1922-09-16-a-i0114") | POLITIQUE | 1922-09-16 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-21-a-i0090","JDG-1922-09-21-a-i0090") | Assemblée de la Société des nations | 1922-09-21 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-08-a-i0046","lematin-1922-08-08-a-i0046") | Une conférence internationale socialiste à Bruxelles | 1922-08-08 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/JDG-1922-09-03-a-i0043","JDG-1922-09-03-a-i0043") | Délégués à la troisième assemblée | 1922-09-03 | JDG; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-24-a-i0056","lematin-1922-08-24-a-i0056") | NOUVELLES EN TROIS LIGNES | 1922-08-24 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/EXP-1922-09-04-a-i0040","EXP-1922-09-04-a-i0040") | ; ;•,;. POLITIQUE | 1922-09-04 | EXP; =HYPERLINK("https://impresso-project.ch/app/article/FZG-1922-09-21-a-i0018","FZG-1922-09-21-a-i0018") | • Neueste Meldunge« » | 1922-09-21 | FZG</f>
-        <v>0</v>
+      <c r="H33" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="I33" t="s">
-        <v>256</v>
+        <v>273</v>
       </c>
       <c r="J33" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K33" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2288,27 +2307,26 @@
       <c r="C34" t="s">
         <v>115</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H34" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-30-a-i0036","lematin-1922-08-30-a-i0036") | La Bulgarie envoie une mission secrète à Moscou | 1922-08-30 | lematin; =HYPERLINK("https://impresso-project.ch/app/article/GDL-1922-08-31-a-i0024","GDL-1922-08-31-a-i0024") | S^a VH &amp; | 1922-08-31 | GDL; =HYPERLINK("https://impresso-project.ch/app/article/lematin-1922-08-31-a-i0068","lematin-1922-08-31-a-i0068") | M. Todoroff n'ira pas à Moscou | 1922-08-31 | lematin</f>
-        <v>0</v>
+      <c r="H34" s="1" t="s">
+        <v>259</v>
       </c>
       <c r="I34" t="s">
-        <v>257</v>
+        <v>274</v>
       </c>
       <c r="J34" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K34" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2321,27 +2339,26 @@
       <c r="C35" t="s">
         <v>116</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="H35" s="2"/>
       <c r="I35" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="J35" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K35" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -2354,21 +2371,20 @@
       <c r="C36" t="s">
         <v>117</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="H36" s="2"/>
       <c r="I36" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="K36" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -2381,27 +2397,26 @@
       <c r="C37" t="s">
         <v>118</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="H37" s="2"/>
       <c r="I37" t="s">
         <v>58</v>
       </c>
       <c r="J37" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K37" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -2414,24 +2429,23 @@
       <c r="C38" t="s">
         <v>119</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H38" s="2"/>
       <c r="I38" t="s">
-        <v>258</v>
+        <v>275</v>
       </c>
       <c r="J38" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="K38" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -2444,24 +2458,23 @@
       <c r="C39" t="s">
         <v>120</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="H39" s="2"/>
       <c r="I39" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="J39" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K39" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2474,27 +2487,26 @@
       <c r="C40" t="s">
         <v>121</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H40" s="2">
-        <f>HYPERLINK("https://impresso-project.ch/app/article/legaulois-1922-09-28-a-i0009","legaulois-1922-09-28-a-i0009") | DANS LE MONDE OFFICIEL | 1922-09-28 | legaulois</f>
-        <v>0</v>
+      <c r="H40" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="I40" t="s">
-        <v>259</v>
+        <v>276</v>
       </c>
       <c r="J40" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K40" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2507,24 +2519,23 @@
       <c r="C41" t="s">
         <v>122</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="H41" s="2"/>
       <c r="I41" t="s">
-        <v>244</v>
+        <v>261</v>
       </c>
       <c r="J41" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="K41" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>